<commit_message>
Ändrade namn på sheet
</commit_message>
<xml_diff>
--- a/manuell_berakning_minimum_kapital.xlsx
+++ b/manuell_berakning_minimum_kapital.xlsx
@@ -9,7 +9,7 @@
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" state="visible" r:id="rId3"/>
-    <sheet name="Blad2" sheetId="2" state="visible" r:id="rId4"/>
+    <sheet name="IG marknader" sheetId="2" state="visible" r:id="rId4"/>
     <sheet name="Norgate tickers" sheetId="3" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="true" iterateDelta="0.001"/>
@@ -1084,6 +1084,7 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -1134,7 +1135,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1239,11 +1240,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -4632,536 +4637,536 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="37.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="26" width="37.18"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="26" t="s">
+    <row r="1" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="27" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="27" t="s">
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="28" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="27" t="s">
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="28" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="27" t="s">
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="28" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="27" t="s">
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="28" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="27" t="s">
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="28" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="27" t="s">
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="28" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="27" t="s">
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="28" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="27" t="s">
+    <row r="9" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="28" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="27" t="s">
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="28" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="27" t="s">
+    <row r="11" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="28" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="27" t="s">
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="28" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="27" t="s">
+    <row r="13" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="28" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="27" t="s">
+    <row r="14" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="28" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="27" t="s">
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="28" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="27" t="s">
+    <row r="16" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="28" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="27" t="s">
+    <row r="17" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="28" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="27" t="s">
+    <row r="18" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="28" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="27" t="s">
+    <row r="19" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="28" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="27" t="s">
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="28" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="27" t="s">
+    <row r="21" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="28" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="27" t="s">
+    <row r="22" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="28" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="27" t="s">
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="28" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="27" t="s">
+    <row r="24" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="28" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="27" t="s">
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="28" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="27" t="s">
+    <row r="26" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="28" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="27" t="s">
+    <row r="27" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="28" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="27" t="s">
+    <row r="28" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="28" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="27" t="s">
+    <row r="29" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="28" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="27" t="s">
+    <row r="30" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="28" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="27" t="s">
+    <row r="31" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="28" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="27" t="s">
+    <row r="32" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="28" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="27" t="s">
+    <row r="33" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="28" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="27" t="s">
+    <row r="34" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="28" t="s">
         <v>270</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="27" t="s">
+    <row r="35" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="28" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="27" t="s">
+    <row r="36" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="28" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="27" t="s">
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="28" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="27" t="s">
+    <row r="38" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="28" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="27" t="s">
+    <row r="39" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="28" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="27" t="s">
+    <row r="40" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="28" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="27" t="s">
+    <row r="41" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="28" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="27" t="s">
+    <row r="42" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="28" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="27" t="s">
+    <row r="43" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="28" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="27" t="s">
+    <row r="44" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="28" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="27" t="s">
+    <row r="45" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="28" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="27" t="s">
+    <row r="46" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="28" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="27" t="s">
+    <row r="47" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="28" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="27" t="s">
+    <row r="48" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="28" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="27" t="s">
+    <row r="49" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="28" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="27" t="s">
+    <row r="50" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="28" t="s">
         <v>284</v>
       </c>
     </row>
-    <row r="51" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="27" t="s">
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="28" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="52" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="27" t="s">
+    <row r="52" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="28" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="27" t="s">
+    <row r="53" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="28" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="54" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="27" t="s">
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="28" t="s">
         <v>288</v>
       </c>
     </row>
-    <row r="55" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="27" t="s">
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="28" t="s">
         <v>289</v>
       </c>
     </row>
-    <row r="56" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="27" t="s">
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="28" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="57" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="27" t="s">
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="28" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="58" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="27" t="s">
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="28" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="59" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="27" t="s">
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="28" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="60" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="27" t="s">
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="28" t="s">
         <v>293</v>
       </c>
     </row>
-    <row r="61" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="27" t="s">
+    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="28" t="s">
         <v>294</v>
       </c>
     </row>
-    <row r="62" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="27" t="s">
+    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="28" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="63" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="27" t="s">
+    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="28" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="64" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="27" t="s">
+    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="28" t="s">
         <v>296</v>
       </c>
     </row>
-    <row r="65" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="27" t="s">
+    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="28" t="s">
         <v>297</v>
       </c>
     </row>
-    <row r="66" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="27" t="s">
+    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="28" t="s">
         <v>298</v>
       </c>
     </row>
-    <row r="67" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="27" t="s">
+    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="28" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="68" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="27" t="s">
+    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="28" t="s">
         <v>300</v>
       </c>
     </row>
-    <row r="69" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="27" t="s">
+    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="28" t="s">
         <v>301</v>
       </c>
     </row>
-    <row r="70" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="27" t="s">
+    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="28" t="s">
         <v>302</v>
       </c>
     </row>
-    <row r="71" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="27" t="s">
+    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="28" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="72" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="27" t="s">
+    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="28" t="s">
         <v>304</v>
       </c>
     </row>
-    <row r="73" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="27" t="s">
+    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A73" s="28" t="s">
         <v>305</v>
       </c>
     </row>
-    <row r="74" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="27" t="s">
+    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A74" s="28" t="s">
         <v>306</v>
       </c>
     </row>
-    <row r="75" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A75" s="27" t="s">
+    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="28" t="s">
         <v>307</v>
       </c>
     </row>
-    <row r="76" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A76" s="27" t="s">
+    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="28" t="s">
         <v>308</v>
       </c>
     </row>
-    <row r="77" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="27" t="s">
+    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A77" s="28" t="s">
         <v>309</v>
       </c>
     </row>
-    <row r="78" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="27" t="s">
+    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="28" t="s">
         <v>310</v>
       </c>
     </row>
-    <row r="79" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="27" t="s">
+    <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A79" s="28" t="s">
         <v>311</v>
       </c>
     </row>
-    <row r="80" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A80" s="27" t="s">
+    <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A80" s="28" t="s">
         <v>312</v>
       </c>
     </row>
-    <row r="81" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A81" s="27" t="s">
+    <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A81" s="28" t="s">
         <v>313</v>
       </c>
     </row>
-    <row r="82" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A82" s="27" t="s">
+    <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A82" s="28" t="s">
         <v>314</v>
       </c>
     </row>
-    <row r="83" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A83" s="27" t="s">
+    <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A83" s="28" t="s">
         <v>315</v>
       </c>
     </row>
-    <row r="84" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A84" s="27" t="s">
+    <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A84" s="28" t="s">
         <v>316</v>
       </c>
     </row>
-    <row r="85" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A85" s="27" t="s">
+    <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A85" s="28" t="s">
         <v>317</v>
       </c>
     </row>
-    <row r="86" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A86" s="27" t="s">
+    <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A86" s="28" t="s">
         <v>318</v>
       </c>
     </row>
-    <row r="87" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A87" s="27" t="s">
+    <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A87" s="28" t="s">
         <v>319</v>
       </c>
     </row>
-    <row r="88" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A88" s="27" t="s">
+    <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A88" s="28" t="s">
         <v>320</v>
       </c>
     </row>
-    <row r="89" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A89" s="27" t="s">
+    <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A89" s="28" t="s">
         <v>321</v>
       </c>
     </row>
-    <row r="90" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A90" s="27" t="s">
+    <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A90" s="28" t="s">
         <v>322</v>
       </c>
     </row>
-    <row r="91" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A91" s="27" t="s">
+    <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A91" s="28" t="s">
         <v>323</v>
       </c>
     </row>
-    <row r="92" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A92" s="27" t="s">
+    <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A92" s="28" t="s">
         <v>324</v>
       </c>
     </row>
-    <row r="93" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A93" s="27" t="s">
+    <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A93" s="28" t="s">
         <v>325</v>
       </c>
     </row>
-    <row r="94" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A94" s="27" t="s">
+    <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A94" s="28" t="s">
         <v>326</v>
       </c>
     </row>
-    <row r="95" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A95" s="27" t="s">
+    <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A95" s="28" t="s">
         <v>327</v>
       </c>
     </row>
-    <row r="96" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A96" s="27" t="s">
+    <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A96" s="28" t="s">
         <v>328</v>
       </c>
     </row>
-    <row r="97" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A97" s="27" t="s">
+    <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A97" s="28" t="s">
         <v>329</v>
       </c>
     </row>
-    <row r="98" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A98" s="27" t="s">
+    <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A98" s="28" t="s">
         <v>330</v>
       </c>
     </row>
-    <row r="99" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A99" s="27" t="s">
+    <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A99" s="28" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="100" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A100" s="27" t="s">
+    <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A100" s="28" t="s">
         <v>331</v>
       </c>
     </row>
-    <row r="101" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A101" s="27" t="s">
+    <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A101" s="28" t="s">
         <v>332</v>
       </c>
     </row>
-    <row r="102" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A102" s="27" t="s">
+    <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A102" s="28" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="103" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A103" s="27" t="s">
+    <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A103" s="28" t="s">
         <v>333</v>
       </c>
     </row>
-    <row r="104" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A104" s="27" t="s">
+    <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A104" s="28" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="105" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A105" s="27" t="s">
+    <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A105" s="28" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="106" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A106" s="27" t="s">
+    <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A106" s="28" t="s">
         <v>334</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Börjat fylla i epics manuellt
</commit_message>
<xml_diff>
--- a/manuell_berakning_minimum_kapital.xlsx
+++ b/manuell_berakning_minimum_kapital.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2">
   <fileVersion appName="Calc"/>
   <workbookPr backupFile="false" showObjects="all" date1904="true"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" state="visible" r:id="rId3"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="458" uniqueCount="335">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="810" uniqueCount="495">
   <si>
     <t xml:space="preserve">Namn</t>
   </si>
@@ -750,300 +750,779 @@
     <t xml:space="preserve">US 30-Day Fed Funds Rate</t>
   </si>
   <si>
+    <t xml:space="preserve">Code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Group</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Epic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Can I trade on IG markets</t>
+  </si>
+  <si>
     <t xml:space="preserve">Australian Dollar</t>
   </si>
   <si>
+    <t xml:space="preserve">6A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Currency</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spot</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CS.D.AUDUSD.CFD.IP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">True</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spot mini</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CS.D.AUDUSD.MINI.IP</t>
+  </si>
+  <si>
     <t xml:space="preserve">British Pound</t>
   </si>
   <si>
+    <t xml:space="preserve">6B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CS.D.GBPUSD.CFD.IP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CS.D.GBPUSD.MINI.IP</t>
+  </si>
+  <si>
     <t xml:space="preserve">Canadian Dollar</t>
   </si>
   <si>
+    <t xml:space="preserve">6C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">False</t>
+  </si>
+  <si>
     <t xml:space="preserve">Euro FX</t>
   </si>
   <si>
+    <t xml:space="preserve">6E</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CS.D.EURUSD.CEE.IP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CS.D.EURUSD.CEEM.IP</t>
+  </si>
+  <si>
     <t xml:space="preserve">Japanese Yen</t>
   </si>
   <si>
+    <t xml:space="preserve">6J</t>
+  </si>
+  <si>
     <t xml:space="preserve">Mexican Peso</t>
   </si>
   <si>
+    <t xml:space="preserve">6M</t>
+  </si>
+  <si>
     <t xml:space="preserve">New Zealand Dollar</t>
   </si>
   <si>
+    <t xml:space="preserve">6N</t>
+  </si>
+  <si>
     <t xml:space="preserve">Swiss Franc</t>
   </si>
   <si>
+    <t xml:space="preserve">6S</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Live Cattle 1€</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Agriculture &amp; Livestock</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CC.D.LC.UME.IP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Live Cattle 4$</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CC.D.LC.UNC.IP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Live Cattle 2$</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CO.D.LC.FWM1.IP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CO.D.LC.FWS1.IP</t>
+  </si>
+  <si>
     <t xml:space="preserve">Feeder Cattle</t>
   </si>
   <si>
+    <t xml:space="preserve">GF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lean Hogs 2$</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CO.D.LH.FWM1.IP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lean Hogs 4$</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CO.D.LH.FWS1.IP</t>
+  </si>
+  <si>
     <t xml:space="preserve">S&amp;P GSCI</t>
   </si>
   <si>
+    <t xml:space="preserve">GD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Commodity Index</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Finns som ETF</t>
+  </si>
+  <si>
     <t xml:space="preserve">Class III Milk</t>
   </si>
   <si>
-    <t xml:space="preserve">Corn</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rough Rice</t>
+    <t xml:space="preserve">DC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Corn 50$</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ZC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CC.D.C.UNC.IP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Corn 1€</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CC.D.C.UME.IP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CO.D.C.FWS2.IP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Corn 25$</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CO.D.C.FWM2.IP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rough Rice 1$</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ZR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CO.D.RR.FWM1.IP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rough Rice 2$</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CO.D.RR.FWS1.IP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Soybean Meal 1$</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ZM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CC.D.SM.UNC.IP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Soybean Meal 1€</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CC.D.SM.UME.IP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CO.D.SM.FWS1.IP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Soybean Meal 0,5$</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CO.D.SM.FWM1.IP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Soybean Oil 6$</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ZL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CC.D.BO.UNC.IP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Soybean Oil 1€</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CC.D.BO.UME.IP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Soybean Oil 3$</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CO.D.BO.FWM1.IP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CO.D.BO.FWS1.IP</t>
   </si>
   <si>
     <t xml:space="preserve">10-Year U.S. T-Note</t>
   </si>
   <si>
+    <t xml:space="preserve">ZN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Interest Rate</t>
+  </si>
+  <si>
     <t xml:space="preserve">E-mini Dow ($5)</t>
   </si>
   <si>
+    <t xml:space="preserve">YM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stock Index</t>
+  </si>
+  <si>
     <t xml:space="preserve">EURO STOXX 50</t>
   </si>
   <si>
+    <t xml:space="preserve">FESX</t>
+  </si>
+  <si>
     <t xml:space="preserve">KOSPI 200</t>
   </si>
   <si>
+    <t xml:space="preserve">KOS</t>
+  </si>
+  <si>
     <t xml:space="preserve">E-mini S&amp;P 500</t>
   </si>
   <si>
+    <t xml:space="preserve">ES</t>
+  </si>
+  <si>
     <t xml:space="preserve">E-mini Nasdaq-100</t>
   </si>
   <si>
+    <t xml:space="preserve">NQ</t>
+  </si>
+  <si>
     <t xml:space="preserve">KC HRW Wheat</t>
   </si>
   <si>
+    <t xml:space="preserve">KE</t>
+  </si>
+  <si>
     <t xml:space="preserve">TecDAX</t>
   </si>
   <si>
+    <t xml:space="preserve">FTDX</t>
+  </si>
+  <si>
     <t xml:space="preserve">Swiss Market Index</t>
   </si>
   <si>
+    <t xml:space="preserve">FSMI</t>
+  </si>
+  <si>
     <t xml:space="preserve">E-mini S&amp;P MidCap 400</t>
   </si>
   <si>
+    <t xml:space="preserve">EMD</t>
+  </si>
+  <si>
     <t xml:space="preserve">Nikkei 225 Dollar</t>
   </si>
   <si>
+    <t xml:space="preserve">NKD</t>
+  </si>
+  <si>
     <t xml:space="preserve">5-Year U.S. T-Note</t>
   </si>
   <si>
+    <t xml:space="preserve">ZF</t>
+  </si>
+  <si>
     <t xml:space="preserve">U.S. T-Bond</t>
   </si>
   <si>
+    <t xml:space="preserve">ZB</t>
+  </si>
+  <si>
     <t xml:space="preserve">2-Year U.S. T-Note</t>
   </si>
   <si>
+    <t xml:space="preserve">ZT</t>
+  </si>
+  <si>
     <t xml:space="preserve">Oats</t>
   </si>
   <si>
+    <t xml:space="preserve">ZO</t>
+  </si>
+  <si>
     <t xml:space="preserve">Chicago SRW Wheat</t>
   </si>
   <si>
+    <t xml:space="preserve">ZW</t>
+  </si>
+  <si>
     <t xml:space="preserve">Soybean</t>
   </si>
   <si>
+    <t xml:space="preserve">ZS</t>
+  </si>
+  <si>
     <t xml:space="preserve">DAX</t>
   </si>
   <si>
+    <t xml:space="preserve">FDAX</t>
+  </si>
+  <si>
     <t xml:space="preserve">Euro-Bund</t>
   </si>
   <si>
+    <t xml:space="preserve">FGBL</t>
+  </si>
+  <si>
     <t xml:space="preserve">Euro-Schatz</t>
   </si>
   <si>
+    <t xml:space="preserve">FGBS</t>
+  </si>
+  <si>
     <t xml:space="preserve">Euro-Bobl</t>
   </si>
   <si>
+    <t xml:space="preserve">FGBM</t>
+  </si>
+  <si>
     <t xml:space="preserve">Euro-Buxl</t>
   </si>
   <si>
+    <t xml:space="preserve">FGBX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LFT</t>
+  </si>
+  <si>
     <t xml:space="preserve">Long Gilt</t>
   </si>
   <si>
+    <t xml:space="preserve">LLG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LEU</t>
+  </si>
+  <si>
     <t xml:space="preserve">CAC 40</t>
   </si>
   <si>
+    <t xml:space="preserve">FCE</t>
+  </si>
+  <si>
     <t xml:space="preserve">London Cocoa</t>
   </si>
   <si>
+    <t xml:space="preserve">LCC</t>
+  </si>
+  <si>
     <t xml:space="preserve">White Sugar</t>
   </si>
   <si>
+    <t xml:space="preserve">LSU</t>
+  </si>
+  <si>
     <t xml:space="preserve">Feed Wheat</t>
   </si>
   <si>
+    <t xml:space="preserve">LWB</t>
+  </si>
+  <si>
     <t xml:space="preserve">Cocoa</t>
   </si>
   <si>
+    <t xml:space="preserve">CC</t>
+  </si>
+  <si>
     <t xml:space="preserve">Coffee C</t>
   </si>
   <si>
+    <t xml:space="preserve">KC</t>
+  </si>
+  <si>
     <t xml:space="preserve">Sugar No. 11</t>
   </si>
   <si>
+    <t xml:space="preserve">SB</t>
+  </si>
+  <si>
     <t xml:space="preserve">Frozen Concentrated Orange Juice Grade A</t>
   </si>
   <si>
+    <t xml:space="preserve">OJ</t>
+  </si>
+  <si>
     <t xml:space="preserve">Cotton No. 2</t>
   </si>
   <si>
+    <t xml:space="preserve">CT</t>
+  </si>
+  <si>
     <t xml:space="preserve">US Dollar Index</t>
   </si>
   <si>
+    <t xml:space="preserve">DX</t>
+  </si>
+  <si>
     <t xml:space="preserve">Crude Oil</t>
   </si>
   <si>
+    <t xml:space="preserve">CL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Energy</t>
+  </si>
+  <si>
     <t xml:space="preserve">NY Harbor ULSD</t>
   </si>
   <si>
+    <t xml:space="preserve">HO</t>
+  </si>
+  <si>
     <t xml:space="preserve">RBOB Gasoline</t>
   </si>
   <si>
+    <t xml:space="preserve">RB</t>
+  </si>
+  <si>
     <t xml:space="preserve">Henry Hub Natural Gas</t>
   </si>
   <si>
+    <t xml:space="preserve">NG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Metal</t>
+  </si>
+  <si>
     <t xml:space="preserve">Platinum</t>
   </si>
   <si>
+    <t xml:space="preserve">PL</t>
+  </si>
+  <si>
     <t xml:space="preserve">Gold</t>
   </si>
   <si>
+    <t xml:space="preserve">GC</t>
+  </si>
+  <si>
     <t xml:space="preserve">Copper</t>
   </si>
   <si>
+    <t xml:space="preserve">HG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SI</t>
+  </si>
+  <si>
     <t xml:space="preserve">Brent Crude Oil</t>
   </si>
   <si>
+    <t xml:space="preserve">BRN</t>
+  </si>
+  <si>
     <t xml:space="preserve">WTI Crude Oil</t>
   </si>
   <si>
+    <t xml:space="preserve">WBS</t>
+  </si>
+  <si>
     <t xml:space="preserve">Low Sulphur Gasoil</t>
   </si>
   <si>
+    <t xml:space="preserve">GAS</t>
+  </si>
+  <si>
     <t xml:space="preserve">10-Year Govt. of Canada Bond</t>
   </si>
   <si>
+    <t xml:space="preserve">CGB</t>
+  </si>
+  <si>
     <t xml:space="preserve">S&amp;P/TSX 60 Index</t>
   </si>
   <si>
+    <t xml:space="preserve">SXF</t>
+  </si>
+  <si>
     <t xml:space="preserve">Canola</t>
   </si>
   <si>
+    <t xml:space="preserve">RS</t>
+  </si>
+  <si>
     <t xml:space="preserve">Hard Red Spring Wheat</t>
   </si>
   <si>
+    <t xml:space="preserve">MWE</t>
+  </si>
+  <si>
     <t xml:space="preserve">Hang Seng Index</t>
   </si>
   <si>
+    <t xml:space="preserve">HSI</t>
+  </si>
+  <si>
     <t xml:space="preserve">Hang Seng Index - Mini</t>
   </si>
   <si>
+    <t xml:space="preserve">MHI</t>
+  </si>
+  <si>
     <t xml:space="preserve">Nikkei 225 (SGX)</t>
   </si>
   <si>
+    <t xml:space="preserve">SNK</t>
+  </si>
+  <si>
     <t xml:space="preserve">MSCI Singapore Index</t>
   </si>
   <si>
+    <t xml:space="preserve">SSG</t>
+  </si>
+  <si>
     <t xml:space="preserve">Japanese Govt Bond - Mini</t>
   </si>
   <si>
+    <t xml:space="preserve">SJB</t>
+  </si>
+  <si>
     <t xml:space="preserve">ASX 90 Day Bank Accepted Bills</t>
   </si>
   <si>
+    <t xml:space="preserve">YIR</t>
+  </si>
+  <si>
     <t xml:space="preserve">ASX 3 Year Treasury Bond</t>
   </si>
   <si>
+    <t xml:space="preserve">YYT</t>
+  </si>
+  <si>
     <t xml:space="preserve">ASX 10 Year Treasury Bond</t>
   </si>
   <si>
+    <t xml:space="preserve">YXT</t>
+  </si>
+  <si>
     <t xml:space="preserve">ASX SPI 200</t>
   </si>
   <si>
+    <t xml:space="preserve">YAP</t>
+  </si>
+  <si>
     <t xml:space="preserve">30 Day Federal Funds</t>
   </si>
   <si>
+    <t xml:space="preserve">ZQ</t>
+  </si>
+  <si>
     <t xml:space="preserve">ASX 30 Day Interbank Cash Rate</t>
   </si>
   <si>
+    <t xml:space="preserve">YIB</t>
+  </si>
+  <si>
     <t xml:space="preserve">Robusta Coffee 10 Tonne</t>
   </si>
   <si>
+    <t xml:space="preserve">LRC</t>
+  </si>
+  <si>
     <t xml:space="preserve">CBOE Volatility Index</t>
   </si>
   <si>
+    <t xml:space="preserve">VX</t>
+  </si>
+  <si>
     <t xml:space="preserve">Ultra U.S. T-Bond</t>
   </si>
   <si>
+    <t xml:space="preserve">UB</t>
+  </si>
+  <si>
     <t xml:space="preserve">Nikkei 225 Yen</t>
   </si>
   <si>
+    <t xml:space="preserve">NIY</t>
+  </si>
+  <si>
     <t xml:space="preserve">Eastern Australia Feed Barley</t>
   </si>
   <si>
+    <t xml:space="preserve">AFB</t>
+  </si>
+  <si>
     <t xml:space="preserve">Euro-BTP Long-Term</t>
   </si>
   <si>
+    <t xml:space="preserve">FBTP</t>
+  </si>
+  <si>
     <t xml:space="preserve">FTSE China A50 Index</t>
   </si>
   <si>
+    <t xml:space="preserve">SCN</t>
+  </si>
+  <si>
     <t xml:space="preserve">UK Natural Gas</t>
   </si>
   <si>
+    <t xml:space="preserve">GWM</t>
+  </si>
+  <si>
     <t xml:space="preserve">EUA</t>
   </si>
   <si>
     <t xml:space="preserve">Euro-OAT</t>
   </si>
   <si>
+    <t xml:space="preserve">FOAT</t>
+  </si>
+  <si>
     <t xml:space="preserve">Eastern Australia Wheat</t>
   </si>
   <si>
+    <t xml:space="preserve">AWM</t>
+  </si>
+  <si>
     <t xml:space="preserve">Ultra 10-Year U.S. T-Note</t>
   </si>
   <si>
+    <t xml:space="preserve">TN</t>
+  </si>
+  <si>
     <t xml:space="preserve">E-mini Russell 2000</t>
   </si>
   <si>
+    <t xml:space="preserve">RTY</t>
+  </si>
+  <si>
     <t xml:space="preserve">Bitcoin</t>
   </si>
   <si>
+    <t xml:space="preserve">BTC</t>
+  </si>
+  <si>
     <t xml:space="preserve">Micro E-mini S&amp;P 500</t>
   </si>
   <si>
+    <t xml:space="preserve">MES</t>
+  </si>
+  <si>
     <t xml:space="preserve">Micro E-mini Nasdaq-100</t>
   </si>
   <si>
+    <t xml:space="preserve">MNQ</t>
+  </si>
+  <si>
     <t xml:space="preserve">Micro E-mini Russell 2000</t>
   </si>
   <si>
+    <t xml:space="preserve">M2K</t>
+  </si>
+  <si>
     <t xml:space="preserve">Micro E-mini Dow Jones Industrial Average</t>
   </si>
   <si>
+    <t xml:space="preserve">MYM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SR3</t>
+  </si>
+  <si>
     <t xml:space="preserve">MSCI Taiwan Index</t>
   </si>
   <si>
+    <t xml:space="preserve">HTW</t>
+  </si>
+  <si>
     <t xml:space="preserve">Micro Bitcoin</t>
   </si>
   <si>
+    <t xml:space="preserve">MBT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ETH</t>
+  </si>
+  <si>
     <t xml:space="preserve">Micro Ether</t>
   </si>
   <si>
+    <t xml:space="preserve">MET</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SO3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LBR</t>
+  </si>
+  <si>
     <t xml:space="preserve">Three-Month CORRA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CRA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="8">
+  <numFmts count="7">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="[$$-409]#,##0.00;[RED]\-[$$-409]#,##0.00"/>
     <numFmt numFmtId="166" formatCode="[$$-409]#,##0;[RED]\-[$$-409]#,##0"/>
     <numFmt numFmtId="167" formatCode="[$-41D]0.00\ %"/>
     <numFmt numFmtId="168" formatCode="0.00\ %"/>
-    <numFmt numFmtId="169" formatCode="General"/>
-    <numFmt numFmtId="170" formatCode="[$$-409]#,##0.0;[RED]\-[$$-409]#,##0.0"/>
-    <numFmt numFmtId="171" formatCode="#,##0.00\ [$€-81D];[RED]\-#,##0.00\ [$€-81D]"/>
+    <numFmt numFmtId="169" formatCode="[$$-409]#,##0.0;[RED]\-[$$-409]#,##0.0"/>
+    <numFmt numFmtId="170" formatCode="#,##0.00\ [$€-81D];[RED]\-#,##0.00\ [$€-81D]"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1085,6 +1564,11 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Liberation Mono;Courier New;DejaVu Sans Mono"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="3">
@@ -1135,7 +1619,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1204,11 +1688,11 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="169" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="170" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="169" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1216,7 +1700,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="171" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="170" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1249,6 +1733,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1438,10 +1926,10 @@
   <dimension ref="A1:T53"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F25" activeCellId="0" sqref="F25"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="1" style="1" width="11.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="4.91"/>
@@ -1554,22 +2042,22 @@
         <v>0.249128091312619</v>
       </c>
       <c r="J2" s="14" t="n">
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
       <c r="K2" s="13" t="n">
         <f aca="false">(H2*I2)/J2*D2</f>
-        <v>209533.333333333</v>
+        <v>314300</v>
       </c>
       <c r="L2" s="13" t="n">
         <f aca="false">K2*4</f>
-        <v>838133.333333334</v>
+        <v>1257200</v>
       </c>
       <c r="M2" s="15" t="n">
         <v>0.05</v>
       </c>
       <c r="N2" s="13" t="n">
         <f aca="false">M2*L2</f>
-        <v>41906.6666666667</v>
+        <v>62860</v>
       </c>
       <c r="O2" s="11" t="n">
         <v>25232</v>
@@ -1625,22 +2113,22 @@
       </c>
       <c r="J3" s="14" t="n">
         <f aca="false">J2</f>
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
       <c r="K3" s="13" t="n">
         <f aca="false">(H3*I3)/J3*D3</f>
-        <v>10476.6666666667</v>
+        <v>15715</v>
       </c>
       <c r="L3" s="13" t="n">
         <f aca="false">K3*4</f>
-        <v>41906.6666666667</v>
+        <v>62860</v>
       </c>
       <c r="M3" s="15" t="n">
         <v>0.05</v>
       </c>
       <c r="N3" s="13" t="n">
         <f aca="false">M3*L3</f>
-        <v>2095.33333333333</v>
+        <v>3143</v>
       </c>
       <c r="O3" s="11" t="n">
         <v>25232</v>
@@ -1696,22 +2184,22 @@
       </c>
       <c r="J4" s="14" t="n">
         <f aca="false">J3</f>
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
       <c r="K4" s="13" t="n">
         <f aca="false">(H4*I4)/J4*D4</f>
-        <v>2095.33333333333</v>
+        <v>3143</v>
       </c>
       <c r="L4" s="13" t="n">
         <f aca="false">K4*4</f>
-        <v>8381.33333333333</v>
+        <v>12572</v>
       </c>
       <c r="M4" s="15" t="n">
         <v>0.05</v>
       </c>
       <c r="N4" s="13" t="n">
         <f aca="false">M4*L4</f>
-        <v>419.066666666667</v>
+        <v>628.600000000001</v>
       </c>
       <c r="O4" s="19" t="n">
         <v>25117.5</v>
@@ -1764,22 +2252,22 @@
       </c>
       <c r="J5" s="14" t="n">
         <f aca="false">J4</f>
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
       <c r="K5" s="13" t="n">
         <f aca="false">(H5*I5)/J5*D5</f>
-        <v>44489.5598466667</v>
+        <v>66734.3397699999</v>
       </c>
       <c r="L5" s="13" t="n">
         <f aca="false">K5*4</f>
-        <v>177958.239386667</v>
+        <v>266937.359079999</v>
       </c>
       <c r="M5" s="15" t="n">
         <v>0.05</v>
       </c>
       <c r="N5" s="13" t="n">
         <f aca="false">M5*L5</f>
-        <v>8897.91196933333</v>
+        <v>13346.867954</v>
       </c>
       <c r="O5" s="11" t="n">
         <v>23844.2</v>
@@ -1887,22 +2375,22 @@
       </c>
       <c r="J8" s="16" t="n">
         <f aca="false">J5</f>
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
       <c r="K8" s="23" t="n">
         <f aca="false">(H8*I8)/J8</f>
-        <v>3266.66666666667</v>
+        <v>4900</v>
       </c>
       <c r="L8" s="23" t="n">
         <f aca="false">K8*4</f>
-        <v>13066.6666666667</v>
+        <v>19600</v>
       </c>
       <c r="M8" s="24" t="n">
         <v>0.05</v>
       </c>
       <c r="N8" s="23" t="n">
         <f aca="false">M8*L8</f>
-        <v>653.333333333333</v>
+        <v>980</v>
       </c>
       <c r="O8" s="21" t="n">
         <v>6738.54</v>
@@ -1955,22 +2443,22 @@
       </c>
       <c r="J9" s="16" t="n">
         <f aca="false">J8</f>
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
       <c r="K9" s="23" t="n">
         <f aca="false">(H9*I9)/J9</f>
-        <v>16333.3333333333</v>
+        <v>24500</v>
       </c>
       <c r="L9" s="23" t="n">
         <f aca="false">K9*4</f>
-        <v>65333.3333333333</v>
+        <v>98000</v>
       </c>
       <c r="M9" s="24" t="n">
         <v>0.05</v>
       </c>
       <c r="N9" s="23" t="n">
         <f aca="false">M9*L9</f>
-        <v>3266.66666666667</v>
+        <v>4900</v>
       </c>
       <c r="O9" s="21" t="n">
         <v>6738.54</v>
@@ -2009,7 +2497,7 @@
       <c r="I10" s="16"/>
       <c r="J10" s="16" t="n">
         <f aca="false">J8</f>
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
       <c r="K10" s="23"/>
       <c r="L10" s="23"/>
@@ -2043,7 +2531,7 @@
       <c r="I11" s="16"/>
       <c r="J11" s="16" t="n">
         <f aca="false">J10</f>
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
       <c r="K11" s="23"/>
       <c r="L11" s="23"/>
@@ -2077,7 +2565,7 @@
       <c r="I12" s="16"/>
       <c r="J12" s="16" t="n">
         <f aca="false">J11</f>
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
       <c r="K12" s="23"/>
       <c r="L12" s="23"/>
@@ -2111,7 +2599,7 @@
       <c r="I13" s="16"/>
       <c r="J13" s="16" t="n">
         <f aca="false">J12</f>
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
       <c r="K13" s="23"/>
       <c r="L13" s="23"/>
@@ -2145,7 +2633,7 @@
       <c r="I14" s="16"/>
       <c r="J14" s="16" t="n">
         <f aca="false">J13</f>
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
       <c r="K14" s="23"/>
       <c r="L14" s="23"/>
@@ -2179,7 +2667,7 @@
       <c r="I15" s="16"/>
       <c r="J15" s="16" t="n">
         <f aca="false">J14</f>
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
       <c r="K15" s="23"/>
       <c r="L15" s="23"/>
@@ -2213,7 +2701,7 @@
       <c r="I16" s="16"/>
       <c r="J16" s="16" t="n">
         <f aca="false">J15</f>
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
       <c r="K16" s="23"/>
       <c r="L16" s="23"/>
@@ -2247,7 +2735,7 @@
       <c r="I17" s="16"/>
       <c r="J17" s="16" t="n">
         <f aca="false">J16</f>
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
       <c r="K17" s="23"/>
       <c r="L17" s="23"/>
@@ -2281,7 +2769,7 @@
       <c r="I18" s="16"/>
       <c r="J18" s="16" t="n">
         <f aca="false">J17</f>
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
       <c r="K18" s="23"/>
       <c r="L18" s="23"/>
@@ -2315,7 +2803,7 @@
       <c r="I19" s="16"/>
       <c r="J19" s="16" t="n">
         <f aca="false">J18</f>
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
       <c r="K19" s="23"/>
       <c r="L19" s="23"/>
@@ -2349,7 +2837,7 @@
       <c r="I20" s="16"/>
       <c r="J20" s="16" t="n">
         <f aca="false">J19</f>
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
       <c r="K20" s="23"/>
       <c r="L20" s="23"/>
@@ -2383,7 +2871,7 @@
       <c r="I21" s="16"/>
       <c r="J21" s="16" t="n">
         <f aca="false">J20</f>
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
       <c r="K21" s="23"/>
       <c r="L21" s="23"/>
@@ -2417,7 +2905,7 @@
       <c r="I22" s="16"/>
       <c r="J22" s="16" t="n">
         <f aca="false">J21</f>
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
       <c r="K22" s="23"/>
       <c r="L22" s="23"/>
@@ -2451,7 +2939,7 @@
       <c r="I23" s="16"/>
       <c r="J23" s="16" t="n">
         <f aca="false">J22</f>
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
       <c r="K23" s="23"/>
       <c r="L23" s="23"/>
@@ -2485,7 +2973,7 @@
       <c r="I24" s="16"/>
       <c r="J24" s="16" t="n">
         <f aca="false">J23</f>
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
       <c r="K24" s="23"/>
       <c r="L24" s="23"/>
@@ -2519,7 +3007,7 @@
       <c r="I25" s="16"/>
       <c r="J25" s="16" t="n">
         <f aca="false">J24</f>
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
       <c r="K25" s="23"/>
       <c r="L25" s="23"/>
@@ -2553,7 +3041,7 @@
       <c r="I26" s="16"/>
       <c r="J26" s="16" t="n">
         <f aca="false">J25</f>
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
       <c r="K26" s="23"/>
       <c r="L26" s="23"/>
@@ -2587,7 +3075,7 @@
       <c r="I27" s="16"/>
       <c r="J27" s="16" t="n">
         <f aca="false">J26</f>
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
       <c r="K27" s="23"/>
       <c r="L27" s="23"/>
@@ -2621,7 +3109,7 @@
       <c r="I28" s="16"/>
       <c r="J28" s="16" t="n">
         <f aca="false">J27</f>
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
       <c r="K28" s="23"/>
       <c r="L28" s="23"/>
@@ -2655,7 +3143,7 @@
       <c r="I29" s="16"/>
       <c r="J29" s="16" t="n">
         <f aca="false">J28</f>
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
       <c r="K29" s="23"/>
       <c r="L29" s="23"/>
@@ -2689,7 +3177,7 @@
       <c r="I30" s="16"/>
       <c r="J30" s="16" t="n">
         <f aca="false">J29</f>
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
       <c r="K30" s="23"/>
       <c r="L30" s="23"/>
@@ -2723,7 +3211,7 @@
       <c r="I31" s="16"/>
       <c r="J31" s="16" t="n">
         <f aca="false">J30</f>
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
       <c r="K31" s="23"/>
       <c r="L31" s="23"/>
@@ -2757,7 +3245,7 @@
       <c r="I32" s="16"/>
       <c r="J32" s="16" t="n">
         <f aca="false">J31</f>
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
       <c r="K32" s="23"/>
       <c r="L32" s="23"/>
@@ -2791,7 +3279,7 @@
       <c r="I33" s="16"/>
       <c r="J33" s="16" t="n">
         <f aca="false">J32</f>
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
       <c r="K33" s="23"/>
       <c r="L33" s="23"/>
@@ -2825,7 +3313,7 @@
       <c r="I34" s="16"/>
       <c r="J34" s="16" t="n">
         <f aca="false">J33</f>
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
       <c r="K34" s="23"/>
       <c r="L34" s="23"/>
@@ -2859,7 +3347,7 @@
       <c r="I35" s="16"/>
       <c r="J35" s="16" t="n">
         <f aca="false">J34</f>
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
       <c r="K35" s="23"/>
       <c r="L35" s="23"/>
@@ -2893,7 +3381,7 @@
       <c r="I36" s="16"/>
       <c r="J36" s="16" t="n">
         <f aca="false">J35</f>
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
       <c r="K36" s="23"/>
       <c r="L36" s="23"/>
@@ -2927,7 +3415,7 @@
       <c r="I37" s="16"/>
       <c r="J37" s="16" t="n">
         <f aca="false">J36</f>
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
       <c r="K37" s="23"/>
       <c r="L37" s="23"/>
@@ -2961,7 +3449,7 @@
       <c r="I38" s="16"/>
       <c r="J38" s="16" t="n">
         <f aca="false">J37</f>
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
       <c r="K38" s="23"/>
       <c r="L38" s="23"/>
@@ -2995,7 +3483,7 @@
       <c r="I39" s="16"/>
       <c r="J39" s="16" t="n">
         <f aca="false">J38</f>
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
       <c r="K39" s="23"/>
       <c r="L39" s="23"/>
@@ -3029,7 +3517,7 @@
       <c r="I40" s="16"/>
       <c r="J40" s="16" t="n">
         <f aca="false">J39</f>
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
       <c r="K40" s="23"/>
       <c r="L40" s="23"/>
@@ -3063,7 +3551,7 @@
       <c r="I41" s="16"/>
       <c r="J41" s="16" t="n">
         <f aca="false">J40</f>
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
       <c r="K41" s="23"/>
       <c r="L41" s="23"/>
@@ -3097,7 +3585,7 @@
       <c r="I42" s="16"/>
       <c r="J42" s="16" t="n">
         <f aca="false">J41</f>
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
       <c r="K42" s="23"/>
       <c r="L42" s="23"/>
@@ -3131,7 +3619,7 @@
       <c r="I43" s="16"/>
       <c r="J43" s="16" t="n">
         <f aca="false">J42</f>
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
       <c r="K43" s="23"/>
       <c r="L43" s="23"/>
@@ -3165,7 +3653,7 @@
       <c r="I44" s="16"/>
       <c r="J44" s="16" t="n">
         <f aca="false">J43</f>
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
       <c r="K44" s="23"/>
       <c r="L44" s="23"/>
@@ -3199,7 +3687,7 @@
       <c r="I45" s="16"/>
       <c r="J45" s="16" t="n">
         <f aca="false">J44</f>
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
       <c r="K45" s="23"/>
       <c r="L45" s="23"/>
@@ -3233,7 +3721,7 @@
       <c r="I46" s="16"/>
       <c r="J46" s="16" t="n">
         <f aca="false">J45</f>
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
       <c r="K46" s="23"/>
       <c r="L46" s="23"/>
@@ -3267,7 +3755,7 @@
       <c r="I47" s="16"/>
       <c r="J47" s="16" t="n">
         <f aca="false">J46</f>
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
       <c r="K47" s="23"/>
       <c r="L47" s="23"/>
@@ -3301,7 +3789,7 @@
       <c r="I48" s="16"/>
       <c r="J48" s="16" t="n">
         <f aca="false">J47</f>
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
       <c r="K48" s="23"/>
       <c r="L48" s="23"/>
@@ -3335,7 +3823,7 @@
       <c r="I49" s="16"/>
       <c r="J49" s="16" t="n">
         <f aca="false">J48</f>
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
       <c r="K49" s="23"/>
       <c r="L49" s="23"/>
@@ -3369,7 +3857,7 @@
       <c r="I50" s="16"/>
       <c r="J50" s="16" t="n">
         <f aca="false">J49</f>
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
       <c r="K50" s="23"/>
       <c r="L50" s="23"/>
@@ -3403,7 +3891,7 @@
       <c r="I51" s="16"/>
       <c r="J51" s="16" t="n">
         <f aca="false">J50</f>
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
       <c r="K51" s="23"/>
       <c r="L51" s="23"/>
@@ -3437,7 +3925,7 @@
       <c r="I52" s="16"/>
       <c r="J52" s="16" t="n">
         <f aca="false">J51</f>
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
       <c r="K52" s="23"/>
       <c r="L52" s="23"/>
@@ -3471,7 +3959,7 @@
       <c r="I53" s="16"/>
       <c r="J53" s="16" t="n">
         <f aca="false">J52</f>
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
       <c r="K53" s="23"/>
       <c r="L53" s="23"/>
@@ -3507,13 +3995,16 @@
   </sheetPr>
   <dimension ref="A1:A220"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A184" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B217" activeCellId="0" sqref="B217"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.92"/>
+  </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -3588,7 +4079,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="25" t="s">
         <v>37</v>
       </c>
@@ -3598,7 +4089,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="25" t="s">
         <v>39</v>
       </c>
@@ -3618,7 +4109,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="25" t="s">
         <v>43</v>
       </c>
@@ -3638,7 +4129,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="25" t="s">
         <v>47</v>
       </c>
@@ -3653,7 +4144,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="25" t="s">
         <v>50</v>
       </c>
@@ -3668,7 +4159,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="25" t="s">
         <v>53</v>
       </c>
@@ -3733,12 +4224,12 @@
         <v>65</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="25" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="25" t="s">
         <v>67</v>
       </c>
@@ -3748,17 +4239,17 @@
         <v>68</v>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="25" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="25" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="25" t="s">
         <v>71</v>
       </c>
@@ -3768,12 +4259,12 @@
         <v>72</v>
       </c>
     </row>
-    <row r="52" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="25" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="25" t="s">
         <v>74</v>
       </c>
@@ -4629,546 +5120,1734 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:A106"/>
+  <dimension ref="A1:G123"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A64" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A72" activeCellId="0" sqref="A72"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F39" activeCellId="0" sqref="F39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="26" width="37.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="26" width="36.91"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="26" width="7.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="26" width="20.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="26" width="20.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="22.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="26" width="22.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="14.09"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="27" t="s">
         <v>0</v>
       </c>
+      <c r="B1" s="28" t="s">
+        <v>242</v>
+      </c>
+      <c r="C1" s="28" t="s">
+        <v>243</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>244</v>
+      </c>
+      <c r="F1" s="28" t="s">
+        <v>245</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="28" t="s">
-        <v>242</v>
+        <v>246</v>
+      </c>
+      <c r="B2" s="28" t="s">
+        <v>247</v>
+      </c>
+      <c r="C2" s="28" t="s">
+        <v>248</v>
+      </c>
+      <c r="D2" s="26" t="s">
+        <v>249</v>
+      </c>
+      <c r="E2" s="29" t="s">
+        <v>250</v>
+      </c>
+      <c r="F2" s="28" t="s">
+        <v>251</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="28" t="s">
-        <v>243</v>
+        <v>246</v>
+      </c>
+      <c r="B3" s="28" t="s">
+        <v>247</v>
+      </c>
+      <c r="C3" s="28" t="s">
+        <v>248</v>
+      </c>
+      <c r="D3" s="26" t="s">
+        <v>252</v>
+      </c>
+      <c r="E3" s="29" t="s">
+        <v>253</v>
+      </c>
+      <c r="F3" s="28" t="s">
+        <v>251</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="28" t="s">
-        <v>244</v>
+        <v>254</v>
+      </c>
+      <c r="B4" s="28" t="s">
+        <v>255</v>
+      </c>
+      <c r="C4" s="28" t="s">
+        <v>248</v>
+      </c>
+      <c r="D4" s="26" t="s">
+        <v>249</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>256</v>
+      </c>
+      <c r="F4" s="28" t="s">
+        <v>251</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="28" t="s">
-        <v>245</v>
+        <v>254</v>
+      </c>
+      <c r="B5" s="28" t="s">
+        <v>255</v>
+      </c>
+      <c r="C5" s="28" t="s">
+        <v>248</v>
+      </c>
+      <c r="D5" s="26" t="s">
+        <v>252</v>
+      </c>
+      <c r="E5" s="0" t="s">
+        <v>257</v>
+      </c>
+      <c r="F5" s="28" t="s">
+        <v>251</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="28" t="s">
-        <v>246</v>
+        <v>258</v>
+      </c>
+      <c r="B6" s="28" t="s">
+        <v>259</v>
+      </c>
+      <c r="C6" s="28" t="s">
+        <v>248</v>
+      </c>
+      <c r="F6" s="28" t="s">
+        <v>260</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="28" t="s">
-        <v>247</v>
+        <v>261</v>
+      </c>
+      <c r="B7" s="28" t="s">
+        <v>262</v>
+      </c>
+      <c r="C7" s="28" t="s">
+        <v>248</v>
+      </c>
+      <c r="D7" s="26" t="s">
+        <v>249</v>
+      </c>
+      <c r="E7" s="0" t="s">
+        <v>263</v>
+      </c>
+      <c r="F7" s="28" t="s">
+        <v>251</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="28" t="s">
+        <v>261</v>
+      </c>
+      <c r="B8" s="28" t="s">
+        <v>262</v>
+      </c>
+      <c r="C8" s="28" t="s">
         <v>248</v>
       </c>
-    </row>
-    <row r="9" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D8" s="26" t="s">
+        <v>252</v>
+      </c>
+      <c r="E8" s="0" t="s">
+        <v>264</v>
+      </c>
+      <c r="F8" s="28" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="28" t="s">
-        <v>249</v>
+        <v>265</v>
+      </c>
+      <c r="B9" s="28" t="s">
+        <v>266</v>
+      </c>
+      <c r="C9" s="28" t="s">
+        <v>248</v>
+      </c>
+      <c r="D9" s="28"/>
+      <c r="F9" s="28" t="s">
+        <v>260</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="28" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>267</v>
+      </c>
+      <c r="B10" s="28" t="s">
+        <v>268</v>
+      </c>
+      <c r="C10" s="28" t="s">
+        <v>248</v>
+      </c>
+      <c r="F10" s="28" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="28" t="s">
-        <v>250</v>
+        <v>269</v>
+      </c>
+      <c r="B11" s="28" t="s">
+        <v>270</v>
+      </c>
+      <c r="C11" s="28" t="s">
+        <v>248</v>
+      </c>
+      <c r="F11" s="28" t="s">
+        <v>260</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="28" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>271</v>
+      </c>
+      <c r="B12" s="28" t="s">
+        <v>272</v>
+      </c>
+      <c r="C12" s="28" t="s">
+        <v>248</v>
+      </c>
+      <c r="F12" s="28" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="28" t="s">
+        <v>273</v>
+      </c>
+      <c r="B13" s="28" t="s">
+        <v>274</v>
+      </c>
+      <c r="C13" s="28" t="s">
+        <v>275</v>
+      </c>
+      <c r="D13" s="26" t="s">
+        <v>23</v>
+      </c>
+      <c r="E13" s="0" t="s">
+        <v>276</v>
+      </c>
+      <c r="F13" s="28" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="28" t="s">
-        <v>252</v>
+        <v>277</v>
+      </c>
+      <c r="B14" s="28" t="s">
+        <v>274</v>
+      </c>
+      <c r="C14" s="28" t="s">
+        <v>275</v>
+      </c>
+      <c r="D14" s="26" t="s">
+        <v>23</v>
+      </c>
+      <c r="E14" s="0" t="s">
+        <v>278</v>
+      </c>
+      <c r="F14" s="28" t="s">
+        <v>251</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="28" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>279</v>
+      </c>
+      <c r="B15" s="28" t="s">
+        <v>274</v>
+      </c>
+      <c r="C15" s="28" t="s">
+        <v>275</v>
+      </c>
+      <c r="D15" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="E15" s="0" t="s">
+        <v>280</v>
+      </c>
+      <c r="F15" s="28" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="28" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>277</v>
+      </c>
+      <c r="B16" s="28" t="s">
+        <v>274</v>
+      </c>
+      <c r="C16" s="28" t="s">
+        <v>275</v>
+      </c>
+      <c r="D16" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="E16" s="0" t="s">
+        <v>281</v>
+      </c>
+      <c r="F16" s="28" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="28" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>282</v>
+      </c>
+      <c r="B17" s="28" t="s">
+        <v>283</v>
+      </c>
+      <c r="C17" s="28" t="s">
+        <v>275</v>
+      </c>
+      <c r="D17" s="28"/>
+      <c r="F17" s="28" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="28" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>284</v>
+      </c>
+      <c r="B18" s="28" t="s">
+        <v>285</v>
+      </c>
+      <c r="C18" s="28" t="s">
+        <v>275</v>
+      </c>
+      <c r="D18" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="E18" s="0" t="s">
+        <v>286</v>
+      </c>
+      <c r="F18" s="28" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="28" t="s">
-        <v>255</v>
+        <v>287</v>
+      </c>
+      <c r="B19" s="28" t="s">
+        <v>285</v>
+      </c>
+      <c r="C19" s="28" t="s">
+        <v>275</v>
+      </c>
+      <c r="D19" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="E19" s="0" t="s">
+        <v>288</v>
+      </c>
+      <c r="F19" s="28" t="s">
+        <v>251</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="28" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>289</v>
+      </c>
+      <c r="B20" s="28" t="s">
+        <v>290</v>
+      </c>
+      <c r="C20" s="28" t="s">
+        <v>291</v>
+      </c>
+      <c r="F20" s="28"/>
+      <c r="G20" s="0" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="28" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>293</v>
+      </c>
+      <c r="B21" s="28" t="s">
+        <v>294</v>
+      </c>
+      <c r="C21" s="28" t="s">
+        <v>275</v>
+      </c>
+      <c r="D21" s="28"/>
+      <c r="F21" s="28" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="28" t="s">
-        <v>258</v>
+        <v>295</v>
+      </c>
+      <c r="B22" s="28" t="s">
+        <v>296</v>
+      </c>
+      <c r="C22" s="28" t="s">
+        <v>275</v>
+      </c>
+      <c r="D22" s="26" t="s">
+        <v>23</v>
+      </c>
+      <c r="E22" s="0" t="s">
+        <v>297</v>
+      </c>
+      <c r="F22" s="28" t="s">
+        <v>251</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="28" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>298</v>
+      </c>
+      <c r="B23" s="28" t="s">
+        <v>296</v>
+      </c>
+      <c r="C23" s="28" t="s">
+        <v>275</v>
+      </c>
+      <c r="D23" s="26" t="s">
+        <v>23</v>
+      </c>
+      <c r="E23" s="0" t="s">
+        <v>299</v>
+      </c>
+      <c r="F23" s="28" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="28" t="s">
-        <v>260</v>
+        <v>295</v>
+      </c>
+      <c r="B24" s="28" t="s">
+        <v>296</v>
+      </c>
+      <c r="C24" s="28" t="s">
+        <v>275</v>
+      </c>
+      <c r="D24" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="E24" s="0" t="s">
+        <v>300</v>
+      </c>
+      <c r="F24" s="28" t="s">
+        <v>251</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="28" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>301</v>
+      </c>
+      <c r="B25" s="28" t="s">
+        <v>296</v>
+      </c>
+      <c r="C25" s="28" t="s">
+        <v>275</v>
+      </c>
+      <c r="D25" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="E25" s="0" t="s">
+        <v>302</v>
+      </c>
+      <c r="F25" s="28" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="28" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>303</v>
+      </c>
+      <c r="B26" s="28" t="s">
+        <v>304</v>
+      </c>
+      <c r="C26" s="28" t="s">
+        <v>275</v>
+      </c>
+      <c r="D26" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="E26" s="0" t="s">
+        <v>305</v>
+      </c>
+      <c r="F26" s="28" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="28" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>306</v>
+      </c>
+      <c r="B27" s="28" t="s">
+        <v>304</v>
+      </c>
+      <c r="C27" s="28" t="s">
+        <v>275</v>
+      </c>
+      <c r="D27" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="E27" s="0" t="s">
+        <v>307</v>
+      </c>
+      <c r="F27" s="28" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="28" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>308</v>
+      </c>
+      <c r="B28" s="28" t="s">
+        <v>309</v>
+      </c>
+      <c r="C28" s="28" t="s">
+        <v>275</v>
+      </c>
+      <c r="D28" s="26" t="s">
+        <v>23</v>
+      </c>
+      <c r="E28" s="0" t="s">
+        <v>310</v>
+      </c>
+      <c r="F28" s="28" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="28" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>311</v>
+      </c>
+      <c r="B29" s="28" t="s">
+        <v>309</v>
+      </c>
+      <c r="C29" s="28" t="s">
+        <v>275</v>
+      </c>
+      <c r="D29" s="26" t="s">
+        <v>23</v>
+      </c>
+      <c r="E29" s="0" t="s">
+        <v>312</v>
+      </c>
+      <c r="F29" s="28" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="28" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>308</v>
+      </c>
+      <c r="B30" s="28" t="s">
+        <v>309</v>
+      </c>
+      <c r="C30" s="28" t="s">
+        <v>275</v>
+      </c>
+      <c r="D30" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="E30" s="0" t="s">
+        <v>313</v>
+      </c>
+      <c r="F30" s="28" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="28" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="32" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>314</v>
+      </c>
+      <c r="B31" s="28" t="s">
+        <v>309</v>
+      </c>
+      <c r="C31" s="28" t="s">
+        <v>275</v>
+      </c>
+      <c r="D31" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="E31" s="0" t="s">
+        <v>315</v>
+      </c>
+      <c r="F31" s="28" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="28" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="33" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>316</v>
+      </c>
+      <c r="B32" s="28" t="s">
+        <v>317</v>
+      </c>
+      <c r="C32" s="28" t="s">
+        <v>275</v>
+      </c>
+      <c r="D32" s="26" t="s">
+        <v>23</v>
+      </c>
+      <c r="E32" s="0" t="s">
+        <v>318</v>
+      </c>
+      <c r="F32" s="28" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="28" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>319</v>
+      </c>
+      <c r="B33" s="28" t="s">
+        <v>317</v>
+      </c>
+      <c r="C33" s="28" t="s">
+        <v>275</v>
+      </c>
+      <c r="D33" s="26" t="s">
+        <v>23</v>
+      </c>
+      <c r="E33" s="0" t="s">
+        <v>320</v>
+      </c>
+      <c r="F33" s="28" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="28" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="35" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>321</v>
+      </c>
+      <c r="B34" s="28" t="s">
+        <v>317</v>
+      </c>
+      <c r="C34" s="28" t="s">
+        <v>275</v>
+      </c>
+      <c r="D34" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="E34" s="0" t="s">
+        <v>322</v>
+      </c>
+      <c r="F34" s="28" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="28" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="36" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>316</v>
+      </c>
+      <c r="B35" s="28" t="s">
+        <v>317</v>
+      </c>
+      <c r="C35" s="28" t="s">
+        <v>275</v>
+      </c>
+      <c r="D35" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="E35" s="0" t="s">
+        <v>323</v>
+      </c>
+      <c r="F35" s="28" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="28" t="s">
-        <v>272</v>
-      </c>
+        <v>324</v>
+      </c>
+      <c r="B36" s="28" t="s">
+        <v>325</v>
+      </c>
+      <c r="C36" s="28" t="s">
+        <v>326</v>
+      </c>
+      <c r="F36" s="28"/>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="28" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="38" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>327</v>
+      </c>
+      <c r="B37" s="28" t="s">
+        <v>328</v>
+      </c>
+      <c r="C37" s="28" t="s">
+        <v>329</v>
+      </c>
+      <c r="F37" s="28"/>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="28" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="39" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>330</v>
+      </c>
+      <c r="B38" s="28" t="s">
+        <v>331</v>
+      </c>
+      <c r="C38" s="28" t="s">
+        <v>329</v>
+      </c>
+      <c r="F38" s="28"/>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="28" t="s">
+        <v>332</v>
+      </c>
+      <c r="B39" s="28" t="s">
+        <v>333</v>
+      </c>
+      <c r="C39" s="28" t="s">
+        <v>329</v>
+      </c>
+      <c r="F39" s="28"/>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="28" t="s">
+        <v>334</v>
+      </c>
+      <c r="B40" s="28" t="s">
+        <v>335</v>
+      </c>
+      <c r="C40" s="28" t="s">
+        <v>329</v>
+      </c>
+      <c r="F40" s="28"/>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="28" t="s">
+        <v>336</v>
+      </c>
+      <c r="B41" s="28" t="s">
+        <v>337</v>
+      </c>
+      <c r="C41" s="28" t="s">
+        <v>329</v>
+      </c>
+      <c r="F41" s="28"/>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="28" t="s">
+        <v>338</v>
+      </c>
+      <c r="B42" s="28" t="s">
+        <v>339</v>
+      </c>
+      <c r="C42" s="28" t="s">
         <v>275</v>
       </c>
-    </row>
-    <row r="40" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="28" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="41" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="28" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="42" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="28" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="43" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F42" s="28"/>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="28" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="44" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>340</v>
+      </c>
+      <c r="B43" s="28" t="s">
+        <v>341</v>
+      </c>
+      <c r="C43" s="28" t="s">
+        <v>329</v>
+      </c>
+      <c r="F43" s="28"/>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="28" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="45" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>342</v>
+      </c>
+      <c r="B44" s="28" t="s">
+        <v>343</v>
+      </c>
+      <c r="C44" s="28" t="s">
+        <v>329</v>
+      </c>
+      <c r="F44" s="28"/>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="28" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="46" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>344</v>
+      </c>
+      <c r="B45" s="28" t="s">
+        <v>345</v>
+      </c>
+      <c r="C45" s="28" t="s">
+        <v>329</v>
+      </c>
+      <c r="F45" s="28"/>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="28" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="47" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>346</v>
+      </c>
+      <c r="B46" s="28" t="s">
+        <v>347</v>
+      </c>
+      <c r="C46" s="28" t="s">
+        <v>329</v>
+      </c>
+      <c r="F46" s="28"/>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="28" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="48" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>348</v>
+      </c>
+      <c r="B47" s="28" t="s">
+        <v>349</v>
+      </c>
+      <c r="C47" s="28" t="s">
+        <v>326</v>
+      </c>
+      <c r="F47" s="28"/>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="28" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="49" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>350</v>
+      </c>
+      <c r="B48" s="28" t="s">
+        <v>351</v>
+      </c>
+      <c r="C48" s="28" t="s">
+        <v>326</v>
+      </c>
+      <c r="F48" s="28"/>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="28" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="50" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>352</v>
+      </c>
+      <c r="B49" s="28" t="s">
+        <v>353</v>
+      </c>
+      <c r="C49" s="28" t="s">
+        <v>326</v>
+      </c>
+      <c r="F49" s="28"/>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="28" t="s">
-        <v>284</v>
-      </c>
+        <v>354</v>
+      </c>
+      <c r="B50" s="28" t="s">
+        <v>355</v>
+      </c>
+      <c r="C50" s="28" t="s">
+        <v>275</v>
+      </c>
+      <c r="F50" s="28"/>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="28" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="52" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>356</v>
+      </c>
+      <c r="B51" s="28" t="s">
+        <v>357</v>
+      </c>
+      <c r="C51" s="28" t="s">
+        <v>275</v>
+      </c>
+      <c r="F51" s="28"/>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="28" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="53" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>358</v>
+      </c>
+      <c r="B52" s="28" t="s">
+        <v>359</v>
+      </c>
+      <c r="C52" s="28" t="s">
+        <v>275</v>
+      </c>
+      <c r="F52" s="28"/>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="28" t="s">
-        <v>287</v>
-      </c>
+        <v>360</v>
+      </c>
+      <c r="B53" s="28" t="s">
+        <v>361</v>
+      </c>
+      <c r="C53" s="28" t="s">
+        <v>329</v>
+      </c>
+      <c r="F53" s="28"/>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="28" t="s">
-        <v>288</v>
-      </c>
+        <v>362</v>
+      </c>
+      <c r="B54" s="28" t="s">
+        <v>363</v>
+      </c>
+      <c r="C54" s="28" t="s">
+        <v>326</v>
+      </c>
+      <c r="F54" s="28"/>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="28" t="s">
-        <v>289</v>
-      </c>
+        <v>364</v>
+      </c>
+      <c r="B55" s="28" t="s">
+        <v>365</v>
+      </c>
+      <c r="C55" s="28" t="s">
+        <v>326</v>
+      </c>
+      <c r="F55" s="28"/>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="28" t="s">
-        <v>290</v>
-      </c>
+        <v>366</v>
+      </c>
+      <c r="B56" s="28" t="s">
+        <v>367</v>
+      </c>
+      <c r="C56" s="28" t="s">
+        <v>326</v>
+      </c>
+      <c r="F56" s="28"/>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="28" t="s">
-        <v>291</v>
-      </c>
+        <v>368</v>
+      </c>
+      <c r="B57" s="28" t="s">
+        <v>369</v>
+      </c>
+      <c r="C57" s="28" t="s">
+        <v>326</v>
+      </c>
+      <c r="F57" s="28"/>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="28" t="s">
-        <v>195</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="B58" s="28" t="s">
+        <v>370</v>
+      </c>
+      <c r="C58" s="28" t="s">
+        <v>329</v>
+      </c>
+      <c r="F58" s="28"/>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="28" t="s">
-        <v>292</v>
-      </c>
+        <v>371</v>
+      </c>
+      <c r="B59" s="28" t="s">
+        <v>372</v>
+      </c>
+      <c r="C59" s="28" t="s">
+        <v>326</v>
+      </c>
+      <c r="F59" s="28"/>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="28" t="s">
-        <v>293</v>
-      </c>
+        <v>240</v>
+      </c>
+      <c r="B60" s="28" t="s">
+        <v>373</v>
+      </c>
+      <c r="C60" s="28" t="s">
+        <v>326</v>
+      </c>
+      <c r="F60" s="28"/>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="28" t="s">
-        <v>294</v>
-      </c>
+        <v>374</v>
+      </c>
+      <c r="B61" s="28" t="s">
+        <v>375</v>
+      </c>
+      <c r="C61" s="28" t="s">
+        <v>329</v>
+      </c>
+      <c r="F61" s="28"/>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="28" t="s">
-        <v>194</v>
-      </c>
+        <v>376</v>
+      </c>
+      <c r="B62" s="28" t="s">
+        <v>377</v>
+      </c>
+      <c r="C62" s="28" t="s">
+        <v>275</v>
+      </c>
+      <c r="F62" s="28"/>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="28" t="s">
-        <v>295</v>
-      </c>
+        <v>378</v>
+      </c>
+      <c r="B63" s="28" t="s">
+        <v>379</v>
+      </c>
+      <c r="C63" s="28" t="s">
+        <v>275</v>
+      </c>
+      <c r="F63" s="28"/>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="28" t="s">
-        <v>296</v>
-      </c>
+        <v>380</v>
+      </c>
+      <c r="B64" s="28" t="s">
+        <v>381</v>
+      </c>
+      <c r="C64" s="28" t="s">
+        <v>275</v>
+      </c>
+      <c r="F64" s="28"/>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="28" t="s">
-        <v>297</v>
-      </c>
+        <v>382</v>
+      </c>
+      <c r="B65" s="28" t="s">
+        <v>383</v>
+      </c>
+      <c r="C65" s="28" t="s">
+        <v>275</v>
+      </c>
+      <c r="F65" s="28"/>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="28" t="s">
-        <v>298</v>
-      </c>
+        <v>384</v>
+      </c>
+      <c r="B66" s="28" t="s">
+        <v>385</v>
+      </c>
+      <c r="C66" s="28" t="s">
+        <v>275</v>
+      </c>
+      <c r="F66" s="28"/>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="28" t="s">
-        <v>299</v>
-      </c>
+        <v>386</v>
+      </c>
+      <c r="B67" s="28" t="s">
+        <v>387</v>
+      </c>
+      <c r="C67" s="28" t="s">
+        <v>275</v>
+      </c>
+      <c r="F67" s="28"/>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="28" t="s">
-        <v>300</v>
-      </c>
+        <v>388</v>
+      </c>
+      <c r="B68" s="28" t="s">
+        <v>389</v>
+      </c>
+      <c r="C68" s="28" t="s">
+        <v>275</v>
+      </c>
+      <c r="F68" s="28"/>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="28" t="s">
-        <v>301</v>
-      </c>
+        <v>390</v>
+      </c>
+      <c r="B69" s="28" t="s">
+        <v>391</v>
+      </c>
+      <c r="C69" s="28" t="s">
+        <v>275</v>
+      </c>
+      <c r="F69" s="28"/>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="28" t="s">
-        <v>302</v>
-      </c>
+        <v>392</v>
+      </c>
+      <c r="B70" s="28" t="s">
+        <v>393</v>
+      </c>
+      <c r="C70" s="28" t="s">
+        <v>248</v>
+      </c>
+      <c r="F70" s="28"/>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="28" t="s">
-        <v>303</v>
-      </c>
+        <v>394</v>
+      </c>
+      <c r="B71" s="28" t="s">
+        <v>395</v>
+      </c>
+      <c r="C71" s="28" t="s">
+        <v>396</v>
+      </c>
+      <c r="F71" s="28"/>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="28" t="s">
-        <v>304</v>
-      </c>
+        <v>397</v>
+      </c>
+      <c r="B72" s="28" t="s">
+        <v>398</v>
+      </c>
+      <c r="C72" s="28" t="s">
+        <v>396</v>
+      </c>
+      <c r="F72" s="28"/>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="28" t="s">
-        <v>305</v>
-      </c>
+        <v>399</v>
+      </c>
+      <c r="B73" s="28" t="s">
+        <v>400</v>
+      </c>
+      <c r="C73" s="28" t="s">
+        <v>396</v>
+      </c>
+      <c r="F73" s="28"/>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="28" t="s">
-        <v>306</v>
-      </c>
+        <v>401</v>
+      </c>
+      <c r="B74" s="28" t="s">
+        <v>402</v>
+      </c>
+      <c r="C74" s="28" t="s">
+        <v>396</v>
+      </c>
+      <c r="F74" s="28"/>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="28" t="s">
-        <v>307</v>
-      </c>
+        <v>195</v>
+      </c>
+      <c r="B75" s="28" t="s">
+        <v>403</v>
+      </c>
+      <c r="C75" s="28" t="s">
+        <v>404</v>
+      </c>
+      <c r="F75" s="28"/>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="28" t="s">
-        <v>308</v>
-      </c>
+        <v>405</v>
+      </c>
+      <c r="B76" s="28" t="s">
+        <v>406</v>
+      </c>
+      <c r="C76" s="28" t="s">
+        <v>404</v>
+      </c>
+      <c r="F76" s="28"/>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="28" t="s">
-        <v>309</v>
-      </c>
+        <v>407</v>
+      </c>
+      <c r="B77" s="28" t="s">
+        <v>408</v>
+      </c>
+      <c r="C77" s="28" t="s">
+        <v>404</v>
+      </c>
+      <c r="F77" s="28"/>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="28" t="s">
-        <v>310</v>
-      </c>
+        <v>409</v>
+      </c>
+      <c r="B78" s="28" t="s">
+        <v>410</v>
+      </c>
+      <c r="C78" s="28" t="s">
+        <v>404</v>
+      </c>
+      <c r="F78" s="28"/>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="28" t="s">
-        <v>311</v>
-      </c>
+        <v>194</v>
+      </c>
+      <c r="B79" s="28" t="s">
+        <v>411</v>
+      </c>
+      <c r="C79" s="28" t="s">
+        <v>404</v>
+      </c>
+      <c r="F79" s="28"/>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="28" t="s">
-        <v>312</v>
-      </c>
+        <v>412</v>
+      </c>
+      <c r="B80" s="28" t="s">
+        <v>413</v>
+      </c>
+      <c r="C80" s="28" t="s">
+        <v>396</v>
+      </c>
+      <c r="F80" s="28"/>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="28" t="s">
-        <v>313</v>
-      </c>
+        <v>414</v>
+      </c>
+      <c r="B81" s="28" t="s">
+        <v>415</v>
+      </c>
+      <c r="C81" s="28" t="s">
+        <v>396</v>
+      </c>
+      <c r="F81" s="28"/>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="28" t="s">
-        <v>314</v>
-      </c>
+        <v>416</v>
+      </c>
+      <c r="B82" s="28" t="s">
+        <v>417</v>
+      </c>
+      <c r="C82" s="28" t="s">
+        <v>396</v>
+      </c>
+      <c r="F82" s="28"/>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="28" t="s">
-        <v>315</v>
-      </c>
+        <v>418</v>
+      </c>
+      <c r="B83" s="28" t="s">
+        <v>419</v>
+      </c>
+      <c r="C83" s="28" t="s">
+        <v>326</v>
+      </c>
+      <c r="F83" s="28"/>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="28" t="s">
-        <v>316</v>
-      </c>
+        <v>420</v>
+      </c>
+      <c r="B84" s="28" t="s">
+        <v>421</v>
+      </c>
+      <c r="C84" s="28" t="s">
+        <v>329</v>
+      </c>
+      <c r="F84" s="28"/>
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="28" t="s">
-        <v>317</v>
-      </c>
+        <v>422</v>
+      </c>
+      <c r="B85" s="28" t="s">
+        <v>423</v>
+      </c>
+      <c r="C85" s="28" t="s">
+        <v>275</v>
+      </c>
+      <c r="F85" s="28"/>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="28" t="s">
-        <v>318</v>
-      </c>
+        <v>424</v>
+      </c>
+      <c r="B86" s="28" t="s">
+        <v>425</v>
+      </c>
+      <c r="C86" s="28" t="s">
+        <v>275</v>
+      </c>
+      <c r="F86" s="28"/>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="28" t="s">
-        <v>319</v>
-      </c>
+        <v>426</v>
+      </c>
+      <c r="B87" s="28" t="s">
+        <v>427</v>
+      </c>
+      <c r="C87" s="28" t="s">
+        <v>329</v>
+      </c>
+      <c r="F87" s="28"/>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="28" t="s">
-        <v>320</v>
-      </c>
+        <v>428</v>
+      </c>
+      <c r="B88" s="28" t="s">
+        <v>429</v>
+      </c>
+      <c r="C88" s="28" t="s">
+        <v>329</v>
+      </c>
+      <c r="F88" s="28"/>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="28" t="s">
-        <v>321</v>
-      </c>
+        <v>430</v>
+      </c>
+      <c r="B89" s="28" t="s">
+        <v>431</v>
+      </c>
+      <c r="C89" s="28" t="s">
+        <v>329</v>
+      </c>
+      <c r="F89" s="28"/>
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="28" t="s">
-        <v>322</v>
-      </c>
+        <v>432</v>
+      </c>
+      <c r="B90" s="28" t="s">
+        <v>433</v>
+      </c>
+      <c r="C90" s="28" t="s">
+        <v>329</v>
+      </c>
+      <c r="F90" s="28"/>
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="28" t="s">
-        <v>323</v>
-      </c>
+        <v>434</v>
+      </c>
+      <c r="B91" s="28" t="s">
+        <v>435</v>
+      </c>
+      <c r="C91" s="28" t="s">
+        <v>326</v>
+      </c>
+      <c r="F91" s="28"/>
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="28" t="s">
-        <v>324</v>
-      </c>
+        <v>436</v>
+      </c>
+      <c r="B92" s="28" t="s">
+        <v>437</v>
+      </c>
+      <c r="C92" s="28" t="s">
+        <v>326</v>
+      </c>
+      <c r="F92" s="28"/>
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="28" t="s">
-        <v>325</v>
-      </c>
+        <v>438</v>
+      </c>
+      <c r="B93" s="28" t="s">
+        <v>439</v>
+      </c>
+      <c r="C93" s="28" t="s">
+        <v>326</v>
+      </c>
+      <c r="F93" s="28"/>
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="28" t="s">
+        <v>440</v>
+      </c>
+      <c r="B94" s="28" t="s">
+        <v>441</v>
+      </c>
+      <c r="C94" s="28" t="s">
         <v>326</v>
       </c>
+      <c r="F94" s="28"/>
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="28" t="s">
-        <v>327</v>
-      </c>
+        <v>442</v>
+      </c>
+      <c r="B95" s="28" t="s">
+        <v>443</v>
+      </c>
+      <c r="C95" s="28" t="s">
+        <v>329</v>
+      </c>
+      <c r="F95" s="28"/>
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="28" t="s">
-        <v>328</v>
-      </c>
+        <v>444</v>
+      </c>
+      <c r="B96" s="28" t="s">
+        <v>445</v>
+      </c>
+      <c r="C96" s="28" t="s">
+        <v>326</v>
+      </c>
+      <c r="F96" s="28"/>
     </row>
     <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="28" t="s">
-        <v>329</v>
-      </c>
+        <v>446</v>
+      </c>
+      <c r="B97" s="28" t="s">
+        <v>447</v>
+      </c>
+      <c r="C97" s="28" t="s">
+        <v>326</v>
+      </c>
+      <c r="F97" s="28"/>
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="28" t="s">
-        <v>330</v>
-      </c>
+        <v>448</v>
+      </c>
+      <c r="B98" s="28" t="s">
+        <v>449</v>
+      </c>
+      <c r="C98" s="28" t="s">
+        <v>275</v>
+      </c>
+      <c r="F98" s="28"/>
     </row>
     <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="28" t="s">
-        <v>237</v>
-      </c>
+        <v>450</v>
+      </c>
+      <c r="B99" s="28" t="s">
+        <v>451</v>
+      </c>
+      <c r="C99" s="28" t="s">
+        <v>329</v>
+      </c>
+      <c r="F99" s="28"/>
     </row>
     <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="28" t="s">
-        <v>331</v>
-      </c>
+        <v>452</v>
+      </c>
+      <c r="B100" s="28" t="s">
+        <v>453</v>
+      </c>
+      <c r="C100" s="28" t="s">
+        <v>326</v>
+      </c>
+      <c r="F100" s="28"/>
     </row>
     <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="28" t="s">
-        <v>332</v>
-      </c>
+        <v>454</v>
+      </c>
+      <c r="B101" s="28" t="s">
+        <v>455</v>
+      </c>
+      <c r="C101" s="28" t="s">
+        <v>329</v>
+      </c>
+      <c r="F101" s="28"/>
     </row>
     <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="28" t="s">
-        <v>168</v>
-      </c>
+        <v>456</v>
+      </c>
+      <c r="B102" s="28" t="s">
+        <v>457</v>
+      </c>
+      <c r="C102" s="28" t="s">
+        <v>275</v>
+      </c>
+      <c r="F102" s="28"/>
     </row>
     <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="28" t="s">
-        <v>333</v>
-      </c>
+        <v>458</v>
+      </c>
+      <c r="B103" s="28" t="s">
+        <v>459</v>
+      </c>
+      <c r="C103" s="28" t="s">
+        <v>326</v>
+      </c>
+      <c r="F103" s="28"/>
     </row>
     <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="28" t="s">
-        <v>238</v>
-      </c>
+        <v>460</v>
+      </c>
+      <c r="B104" s="28" t="s">
+        <v>461</v>
+      </c>
+      <c r="C104" s="28" t="s">
+        <v>329</v>
+      </c>
+      <c r="F104" s="28"/>
     </row>
     <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="28" t="s">
-        <v>217</v>
-      </c>
+        <v>462</v>
+      </c>
+      <c r="B105" s="28" t="s">
+        <v>463</v>
+      </c>
+      <c r="C105" s="28" t="s">
+        <v>396</v>
+      </c>
+      <c r="F105" s="28"/>
     </row>
     <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="28" t="s">
-        <v>334</v>
-      </c>
+        <v>464</v>
+      </c>
+      <c r="B106" s="28" t="s">
+        <v>464</v>
+      </c>
+      <c r="C106" s="28" t="s">
+        <v>291</v>
+      </c>
+      <c r="F106" s="28"/>
+    </row>
+    <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A107" s="28" t="s">
+        <v>465</v>
+      </c>
+      <c r="B107" s="28" t="s">
+        <v>466</v>
+      </c>
+      <c r="C107" s="28" t="s">
+        <v>326</v>
+      </c>
+      <c r="F107" s="28"/>
+    </row>
+    <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A108" s="28" t="s">
+        <v>467</v>
+      </c>
+      <c r="B108" s="28" t="s">
+        <v>468</v>
+      </c>
+      <c r="C108" s="28" t="s">
+        <v>275</v>
+      </c>
+      <c r="F108" s="28"/>
+    </row>
+    <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A109" s="28" t="s">
+        <v>469</v>
+      </c>
+      <c r="B109" s="28" t="s">
+        <v>470</v>
+      </c>
+      <c r="C109" s="28" t="s">
+        <v>326</v>
+      </c>
+      <c r="F109" s="28"/>
+    </row>
+    <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A110" s="28" t="s">
+        <v>471</v>
+      </c>
+      <c r="B110" s="28" t="s">
+        <v>472</v>
+      </c>
+      <c r="C110" s="28" t="s">
+        <v>329</v>
+      </c>
+      <c r="F110" s="28"/>
+    </row>
+    <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A111" s="28" t="s">
+        <v>473</v>
+      </c>
+      <c r="B111" s="28" t="s">
+        <v>474</v>
+      </c>
+      <c r="C111" s="28" t="s">
+        <v>248</v>
+      </c>
+      <c r="F111" s="28"/>
+    </row>
+    <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A112" s="28" t="s">
+        <v>475</v>
+      </c>
+      <c r="B112" s="28" t="s">
+        <v>476</v>
+      </c>
+      <c r="C112" s="28" t="s">
+        <v>329</v>
+      </c>
+      <c r="F112" s="28"/>
+    </row>
+    <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A113" s="28" t="s">
+        <v>477</v>
+      </c>
+      <c r="B113" s="28" t="s">
+        <v>478</v>
+      </c>
+      <c r="C113" s="28" t="s">
+        <v>329</v>
+      </c>
+      <c r="F113" s="28"/>
+    </row>
+    <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A114" s="28" t="s">
+        <v>479</v>
+      </c>
+      <c r="B114" s="28" t="s">
+        <v>480</v>
+      </c>
+      <c r="C114" s="28" t="s">
+        <v>329</v>
+      </c>
+      <c r="F114" s="28"/>
+    </row>
+    <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A115" s="28" t="s">
+        <v>481</v>
+      </c>
+      <c r="B115" s="28" t="s">
+        <v>482</v>
+      </c>
+      <c r="C115" s="28" t="s">
+        <v>329</v>
+      </c>
+      <c r="F115" s="28"/>
+    </row>
+    <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A116" s="28" t="s">
+        <v>237</v>
+      </c>
+      <c r="B116" s="28" t="s">
+        <v>483</v>
+      </c>
+      <c r="C116" s="28" t="s">
+        <v>326</v>
+      </c>
+      <c r="F116" s="28"/>
+    </row>
+    <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A117" s="28" t="s">
+        <v>484</v>
+      </c>
+      <c r="B117" s="28" t="s">
+        <v>485</v>
+      </c>
+      <c r="C117" s="28" t="s">
+        <v>329</v>
+      </c>
+      <c r="F117" s="28"/>
+    </row>
+    <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A118" s="28" t="s">
+        <v>486</v>
+      </c>
+      <c r="B118" s="28" t="s">
+        <v>487</v>
+      </c>
+      <c r="C118" s="28" t="s">
+        <v>248</v>
+      </c>
+      <c r="F118" s="28"/>
+    </row>
+    <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A119" s="28" t="s">
+        <v>168</v>
+      </c>
+      <c r="B119" s="28" t="s">
+        <v>488</v>
+      </c>
+      <c r="C119" s="28" t="s">
+        <v>248</v>
+      </c>
+      <c r="F119" s="28"/>
+    </row>
+    <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A120" s="28" t="s">
+        <v>489</v>
+      </c>
+      <c r="B120" s="28" t="s">
+        <v>490</v>
+      </c>
+      <c r="C120" s="28" t="s">
+        <v>248</v>
+      </c>
+      <c r="F120" s="28"/>
+    </row>
+    <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A121" s="28" t="s">
+        <v>238</v>
+      </c>
+      <c r="B121" s="28" t="s">
+        <v>491</v>
+      </c>
+      <c r="C121" s="28" t="s">
+        <v>326</v>
+      </c>
+      <c r="F121" s="28"/>
+    </row>
+    <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A122" s="28" t="s">
+        <v>217</v>
+      </c>
+      <c r="B122" s="28" t="s">
+        <v>492</v>
+      </c>
+      <c r="C122" s="28" t="s">
+        <v>275</v>
+      </c>
+      <c r="F122" s="28"/>
+    </row>
+    <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A123" s="28" t="s">
+        <v>493</v>
+      </c>
+      <c r="B123" s="28" t="s">
+        <v>494</v>
+      </c>
+      <c r="C123" s="28" t="s">
+        <v>326</v>
+      </c>
+      <c r="F123" s="28"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
Fortsatt att lägga till detaljer kontrakt hos IG markets
</commit_message>
<xml_diff>
--- a/manuell_berakning_minimum_kapital.xlsx
+++ b/manuell_berakning_minimum_kapital.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="810" uniqueCount="495">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="907" uniqueCount="523">
   <si>
     <t xml:space="preserve">Namn</t>
   </si>
@@ -780,9 +780,6 @@
     <t xml:space="preserve">True</t>
   </si>
   <si>
-    <t xml:space="preserve">Spot mini</t>
-  </si>
-  <si>
     <t xml:space="preserve">CS.D.AUDUSD.MINI.IP</t>
   </si>
   <si>
@@ -996,7 +993,7 @@
     <t xml:space="preserve">CO.D.BO.FWS1.IP</t>
   </si>
   <si>
-    <t xml:space="preserve">10-Year U.S. T-Note</t>
+    <t xml:space="preserve">10-Year U.S. T-Note 10$</t>
   </si>
   <si>
     <t xml:space="preserve">ZN</t>
@@ -1005,7 +1002,16 @@
     <t xml:space="preserve">Interest Rate</t>
   </si>
   <si>
-    <t xml:space="preserve">E-mini Dow ($5)</t>
+    <t xml:space="preserve">IR.D.10YEAR100.FWS2.IP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10-Year U.S. T-Note 2$</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IR.D.10YEAR100.FWM2.IP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E-mini Dow 1€</t>
   </si>
   <si>
     <t xml:space="preserve">YM</t>
@@ -1014,28 +1020,106 @@
     <t xml:space="preserve">Stock Index</t>
   </si>
   <si>
-    <t xml:space="preserve">EURO STOXX 50</t>
+    <t xml:space="preserve">IX.D.DOW.INE.IP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E-mini Dow 1$</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IX.D.DOW.IEE.IP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E-mini Dow 2$</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IX.D.DOW.FWM2.IP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E-mini Dow 10$</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IX.D.DOW.FWS2.IP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EURO STOXX 50 2€</t>
   </si>
   <si>
     <t xml:space="preserve">FESX</t>
   </si>
   <si>
+    <t xml:space="preserve">IX.D.STXE.IFM.IP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EURO STOXX 50 10€</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IX.D.STXE.IFD.IP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IX.D.STXE.FWM4.IP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IX.D.STXE.FWS4.IP</t>
+  </si>
+  <si>
     <t xml:space="preserve">KOSPI 200</t>
   </si>
   <si>
     <t xml:space="preserve">KOS</t>
   </si>
   <si>
-    <t xml:space="preserve">E-mini S&amp;P 500</t>
+    <t xml:space="preserve">E-mini S&amp;P 500 1$</t>
   </si>
   <si>
     <t xml:space="preserve">ES</t>
   </si>
   <si>
-    <t xml:space="preserve">E-mini Nasdaq-100</t>
+    <t xml:space="preserve">IX.D.SPTRD.IEE.IP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E-mini S&amp;P 500 1€</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IX.D.SPTRD.INE.IP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E-mini S&amp;P 500 250$</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IX.D.SPTRD.FWS1.IP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E-mini S&amp;P 500 50$</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IX.D.SPTRD.FWM1.IP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E-mini Nasdaq-100 1€</t>
   </si>
   <si>
     <t xml:space="preserve">NQ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IX.D.NASDAQ.INE.IP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E-mini Nasdaq-100 1$</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IX.D.NASDAQ.IEE.IP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E-mini Nasdaq-100 100$</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IX.D.NASDAQ.FWS1.IP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E-mini Nasdaq-100 20$</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IX.D.NASDAQ.FWM1.IP</t>
   </si>
   <si>
     <t xml:space="preserve">KC HRW Wheat</t>
@@ -5120,10 +5204,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G123"/>
+  <dimension ref="A1:G136"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F39" activeCellId="0" sqref="F39"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A46" activeCellId="0" sqref="A46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5188,10 +5272,10 @@
         <v>248</v>
       </c>
       <c r="D3" s="26" t="s">
+        <v>249</v>
+      </c>
+      <c r="E3" s="29" t="s">
         <v>252</v>
-      </c>
-      <c r="E3" s="29" t="s">
-        <v>253</v>
       </c>
       <c r="F3" s="28" t="s">
         <v>251</v>
@@ -5199,10 +5283,10 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="28" t="s">
+        <v>253</v>
+      </c>
+      <c r="B4" s="28" t="s">
         <v>254</v>
-      </c>
-      <c r="B4" s="28" t="s">
-        <v>255</v>
       </c>
       <c r="C4" s="28" t="s">
         <v>248</v>
@@ -5211,7 +5295,7 @@
         <v>249</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F4" s="28" t="s">
         <v>251</v>
@@ -5219,19 +5303,19 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="28" t="s">
+        <v>253</v>
+      </c>
+      <c r="B5" s="28" t="s">
         <v>254</v>
-      </c>
-      <c r="B5" s="28" t="s">
-        <v>255</v>
       </c>
       <c r="C5" s="28" t="s">
         <v>248</v>
       </c>
       <c r="D5" s="26" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="F5" s="28" t="s">
         <v>251</v>
@@ -5239,24 +5323,24 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="28" t="s">
+        <v>257</v>
+      </c>
+      <c r="B6" s="28" t="s">
         <v>258</v>
-      </c>
-      <c r="B6" s="28" t="s">
-        <v>259</v>
       </c>
       <c r="C6" s="28" t="s">
         <v>248</v>
       </c>
       <c r="F6" s="28" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="28" t="s">
+        <v>260</v>
+      </c>
+      <c r="B7" s="28" t="s">
         <v>261</v>
-      </c>
-      <c r="B7" s="28" t="s">
-        <v>262</v>
       </c>
       <c r="C7" s="28" t="s">
         <v>248</v>
@@ -5265,7 +5349,7 @@
         <v>249</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="F7" s="28" t="s">
         <v>251</v>
@@ -5273,19 +5357,19 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="28" t="s">
+        <v>260</v>
+      </c>
+      <c r="B8" s="28" t="s">
         <v>261</v>
-      </c>
-      <c r="B8" s="28" t="s">
-        <v>262</v>
       </c>
       <c r="C8" s="28" t="s">
         <v>248</v>
       </c>
       <c r="D8" s="26" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="F8" s="28" t="s">
         <v>251</v>
@@ -5293,76 +5377,76 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="28" t="s">
+        <v>264</v>
+      </c>
+      <c r="B9" s="28" t="s">
         <v>265</v>
-      </c>
-      <c r="B9" s="28" t="s">
-        <v>266</v>
       </c>
       <c r="C9" s="28" t="s">
         <v>248</v>
       </c>
       <c r="D9" s="28"/>
       <c r="F9" s="28" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="28" t="s">
+        <v>266</v>
+      </c>
+      <c r="B10" s="28" t="s">
         <v>267</v>
-      </c>
-      <c r="B10" s="28" t="s">
-        <v>268</v>
       </c>
       <c r="C10" s="28" t="s">
         <v>248</v>
       </c>
       <c r="F10" s="28" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="28" t="s">
+        <v>268</v>
+      </c>
+      <c r="B11" s="28" t="s">
         <v>269</v>
-      </c>
-      <c r="B11" s="28" t="s">
-        <v>270</v>
       </c>
       <c r="C11" s="28" t="s">
         <v>248</v>
       </c>
       <c r="F11" s="28" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="28" t="s">
+        <v>270</v>
+      </c>
+      <c r="B12" s="28" t="s">
         <v>271</v>
-      </c>
-      <c r="B12" s="28" t="s">
-        <v>272</v>
       </c>
       <c r="C12" s="28" t="s">
         <v>248</v>
       </c>
       <c r="F12" s="28" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="28" t="s">
+        <v>272</v>
+      </c>
+      <c r="B13" s="28" t="s">
         <v>273</v>
       </c>
-      <c r="B13" s="28" t="s">
+      <c r="C13" s="28" t="s">
         <v>274</v>
-      </c>
-      <c r="C13" s="28" t="s">
-        <v>275</v>
       </c>
       <c r="D13" s="26" t="s">
         <v>23</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="F13" s="28" t="s">
         <v>251</v>
@@ -5370,19 +5454,19 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="28" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B14" s="28" t="s">
+        <v>273</v>
+      </c>
+      <c r="C14" s="28" t="s">
         <v>274</v>
-      </c>
-      <c r="C14" s="28" t="s">
-        <v>275</v>
       </c>
       <c r="D14" s="26" t="s">
         <v>23</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="F14" s="28" t="s">
         <v>251</v>
@@ -5390,19 +5474,19 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="28" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B15" s="28" t="s">
+        <v>273</v>
+      </c>
+      <c r="C15" s="28" t="s">
         <v>274</v>
-      </c>
-      <c r="C15" s="28" t="s">
-        <v>275</v>
       </c>
       <c r="D15" s="26" t="s">
         <v>21</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="F15" s="28" t="s">
         <v>251</v>
@@ -5410,19 +5494,19 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="28" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B16" s="28" t="s">
+        <v>273</v>
+      </c>
+      <c r="C16" s="28" t="s">
         <v>274</v>
-      </c>
-      <c r="C16" s="28" t="s">
-        <v>275</v>
       </c>
       <c r="D16" s="26" t="s">
         <v>21</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="F16" s="28" t="s">
         <v>251</v>
@@ -5430,34 +5514,34 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="28" t="s">
+        <v>281</v>
+      </c>
+      <c r="B17" s="28" t="s">
         <v>282</v>
       </c>
-      <c r="B17" s="28" t="s">
-        <v>283</v>
-      </c>
       <c r="C17" s="28" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D17" s="28"/>
       <c r="F17" s="28" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="28" t="s">
+        <v>283</v>
+      </c>
+      <c r="B18" s="28" t="s">
         <v>284</v>
       </c>
-      <c r="B18" s="28" t="s">
-        <v>285</v>
-      </c>
       <c r="C18" s="28" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D18" s="26" t="s">
         <v>21</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="F18" s="28" t="s">
         <v>251</v>
@@ -5465,19 +5549,19 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="28" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B19" s="28" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C19" s="28" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D19" s="26" t="s">
         <v>21</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="F19" s="28" t="s">
         <v>251</v>
@@ -5485,49 +5569,51 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="28" t="s">
+        <v>288</v>
+      </c>
+      <c r="B20" s="28" t="s">
         <v>289</v>
       </c>
-      <c r="B20" s="28" t="s">
+      <c r="C20" s="28" t="s">
         <v>290</v>
       </c>
-      <c r="C20" s="28" t="s">
+      <c r="F20" s="28" t="s">
+        <v>259</v>
+      </c>
+      <c r="G20" s="0" t="s">
         <v>291</v>
-      </c>
-      <c r="F20" s="28"/>
-      <c r="G20" s="0" t="s">
-        <v>292</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="28" t="s">
+        <v>292</v>
+      </c>
+      <c r="B21" s="28" t="s">
         <v>293</v>
       </c>
-      <c r="B21" s="28" t="s">
-        <v>294</v>
-      </c>
       <c r="C21" s="28" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D21" s="28"/>
       <c r="F21" s="28" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="28" t="s">
+        <v>294</v>
+      </c>
+      <c r="B22" s="28" t="s">
         <v>295</v>
       </c>
-      <c r="B22" s="28" t="s">
-        <v>296</v>
-      </c>
       <c r="C22" s="28" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D22" s="26" t="s">
         <v>23</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="F22" s="28" t="s">
         <v>251</v>
@@ -5535,19 +5621,19 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="28" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B23" s="28" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C23" s="28" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D23" s="26" t="s">
         <v>23</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="F23" s="28" t="s">
         <v>251</v>
@@ -5555,19 +5641,19 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="28" t="s">
+        <v>294</v>
+      </c>
+      <c r="B24" s="28" t="s">
         <v>295</v>
       </c>
-      <c r="B24" s="28" t="s">
-        <v>296</v>
-      </c>
       <c r="C24" s="28" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D24" s="26" t="s">
         <v>21</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="F24" s="28" t="s">
         <v>251</v>
@@ -5575,19 +5661,19 @@
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="28" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B25" s="28" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C25" s="28" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D25" s="26" t="s">
         <v>21</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="F25" s="28" t="s">
         <v>251</v>
@@ -5595,19 +5681,19 @@
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="28" t="s">
+        <v>302</v>
+      </c>
+      <c r="B26" s="28" t="s">
         <v>303</v>
       </c>
-      <c r="B26" s="28" t="s">
-        <v>304</v>
-      </c>
       <c r="C26" s="28" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D26" s="26" t="s">
         <v>21</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="F26" s="28" t="s">
         <v>251</v>
@@ -5615,19 +5701,19 @@
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="28" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B27" s="28" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C27" s="28" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D27" s="26" t="s">
         <v>21</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="F27" s="28" t="s">
         <v>251</v>
@@ -5635,19 +5721,19 @@
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="28" t="s">
+        <v>307</v>
+      </c>
+      <c r="B28" s="28" t="s">
         <v>308</v>
       </c>
-      <c r="B28" s="28" t="s">
-        <v>309</v>
-      </c>
       <c r="C28" s="28" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D28" s="26" t="s">
         <v>23</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="F28" s="28" t="s">
         <v>251</v>
@@ -5655,19 +5741,19 @@
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="28" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B29" s="28" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C29" s="28" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D29" s="26" t="s">
         <v>23</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="F29" s="28" t="s">
         <v>251</v>
@@ -5675,19 +5761,19 @@
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="28" t="s">
+        <v>307</v>
+      </c>
+      <c r="B30" s="28" t="s">
         <v>308</v>
       </c>
-      <c r="B30" s="28" t="s">
-        <v>309</v>
-      </c>
       <c r="C30" s="28" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D30" s="26" t="s">
         <v>21</v>
       </c>
       <c r="E30" s="0" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="F30" s="28" t="s">
         <v>251</v>
@@ -5695,19 +5781,19 @@
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="28" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B31" s="28" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C31" s="28" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D31" s="26" t="s">
         <v>21</v>
       </c>
       <c r="E31" s="0" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="F31" s="28" t="s">
         <v>251</v>
@@ -5715,19 +5801,19 @@
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="28" t="s">
+        <v>315</v>
+      </c>
+      <c r="B32" s="28" t="s">
         <v>316</v>
       </c>
-      <c r="B32" s="28" t="s">
-        <v>317</v>
-      </c>
       <c r="C32" s="28" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D32" s="26" t="s">
         <v>23</v>
       </c>
       <c r="E32" s="0" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="F32" s="28" t="s">
         <v>251</v>
@@ -5735,19 +5821,19 @@
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="28" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B33" s="28" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C33" s="28" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D33" s="26" t="s">
         <v>23</v>
       </c>
       <c r="E33" s="0" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="F33" s="28" t="s">
         <v>251</v>
@@ -5755,19 +5841,19 @@
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="28" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B34" s="28" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C34" s="28" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D34" s="26" t="s">
         <v>21</v>
       </c>
       <c r="E34" s="0" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="F34" s="28" t="s">
         <v>251</v>
@@ -5775,19 +5861,19 @@
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="28" t="s">
+        <v>315</v>
+      </c>
+      <c r="B35" s="28" t="s">
         <v>316</v>
       </c>
-      <c r="B35" s="28" t="s">
-        <v>317</v>
-      </c>
       <c r="C35" s="28" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D35" s="26" t="s">
         <v>21</v>
       </c>
       <c r="E35" s="0" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="F35" s="28" t="s">
         <v>251</v>
@@ -5795,123 +5881,203 @@
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="28" t="s">
+        <v>323</v>
+      </c>
+      <c r="B36" s="28" t="s">
         <v>324</v>
       </c>
-      <c r="B36" s="28" t="s">
+      <c r="C36" s="28" t="s">
         <v>325</v>
       </c>
-      <c r="C36" s="28" t="s">
+      <c r="D36" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="E36" s="0" t="s">
         <v>326</v>
       </c>
-      <c r="F36" s="28"/>
+      <c r="F36" s="28" t="s">
+        <v>251</v>
+      </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="28" t="s">
         <v>327</v>
       </c>
       <c r="B37" s="28" t="s">
+        <v>324</v>
+      </c>
+      <c r="C37" s="28" t="s">
+        <v>325</v>
+      </c>
+      <c r="D37" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="E37" s="0" t="s">
         <v>328</v>
       </c>
-      <c r="C37" s="28" t="s">
-        <v>329</v>
-      </c>
-      <c r="F37" s="28"/>
+      <c r="F37" s="28" t="s">
+        <v>251</v>
+      </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="28" t="s">
+        <v>329</v>
+      </c>
+      <c r="B38" s="28" t="s">
         <v>330</v>
       </c>
-      <c r="B38" s="28" t="s">
+      <c r="C38" s="28" t="s">
         <v>331</v>
       </c>
-      <c r="C38" s="28" t="s">
-        <v>329</v>
-      </c>
-      <c r="F38" s="28"/>
+      <c r="D38" s="26" t="s">
+        <v>23</v>
+      </c>
+      <c r="E38" s="0" t="s">
+        <v>332</v>
+      </c>
+      <c r="F38" s="28" t="s">
+        <v>251</v>
+      </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="28" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="B39" s="28" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="C39" s="28" t="s">
-        <v>329</v>
-      </c>
-      <c r="F39" s="28"/>
+        <v>331</v>
+      </c>
+      <c r="D39" s="26" t="s">
+        <v>23</v>
+      </c>
+      <c r="E39" s="0" t="s">
+        <v>334</v>
+      </c>
+      <c r="F39" s="28" t="s">
+        <v>251</v>
+      </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="28" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="B40" s="28" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
       <c r="C40" s="28" t="s">
-        <v>329</v>
-      </c>
-      <c r="F40" s="28"/>
+        <v>331</v>
+      </c>
+      <c r="D40" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="E40" s="0" t="s">
+        <v>336</v>
+      </c>
+      <c r="F40" s="28" t="s">
+        <v>251</v>
+      </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="28" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="B41" s="28" t="s">
-        <v>337</v>
+        <v>330</v>
       </c>
       <c r="C41" s="28" t="s">
-        <v>329</v>
-      </c>
-      <c r="F41" s="28"/>
+        <v>331</v>
+      </c>
+      <c r="D41" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="E41" s="0" t="s">
+        <v>338</v>
+      </c>
+      <c r="F41" s="28" t="s">
+        <v>251</v>
+      </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="28" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="B42" s="28" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="C42" s="28" t="s">
-        <v>275</v>
-      </c>
-      <c r="F42" s="28"/>
+        <v>331</v>
+      </c>
+      <c r="D42" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="E42" s="0" t="s">
+        <v>341</v>
+      </c>
+      <c r="F42" s="28" t="s">
+        <v>251</v>
+      </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="28" t="s">
+        <v>342</v>
+      </c>
+      <c r="B43" s="28" t="s">
         <v>340</v>
       </c>
-      <c r="B43" s="28" t="s">
-        <v>341</v>
-      </c>
       <c r="C43" s="28" t="s">
-        <v>329</v>
-      </c>
-      <c r="F43" s="28"/>
+        <v>331</v>
+      </c>
+      <c r="D43" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="E43" s="0" t="s">
+        <v>343</v>
+      </c>
+      <c r="F43" s="28" t="s">
+        <v>251</v>
+      </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="28" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="B44" s="28" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="C44" s="28" t="s">
-        <v>329</v>
-      </c>
-      <c r="F44" s="28"/>
+        <v>331</v>
+      </c>
+      <c r="D44" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="E44" s="0" t="s">
+        <v>344</v>
+      </c>
+      <c r="F44" s="28" t="s">
+        <v>251</v>
+      </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="28" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="B45" s="28" t="s">
+        <v>340</v>
+      </c>
+      <c r="C45" s="28" t="s">
+        <v>331</v>
+      </c>
+      <c r="D45" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="E45" s="0" t="s">
         <v>345</v>
       </c>
-      <c r="C45" s="28" t="s">
-        <v>329</v>
-      </c>
-      <c r="F45" s="28"/>
+      <c r="F45" s="28" t="s">
+        <v>251</v>
+      </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="28" t="s">
@@ -5921,9 +6087,11 @@
         <v>347</v>
       </c>
       <c r="C46" s="28" t="s">
-        <v>329</v>
-      </c>
-      <c r="F46" s="28"/>
+        <v>331</v>
+      </c>
+      <c r="F46" s="28" t="s">
+        <v>259</v>
+      </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="28" t="s">
@@ -5933,921 +6101,1145 @@
         <v>349</v>
       </c>
       <c r="C47" s="28" t="s">
-        <v>326</v>
-      </c>
-      <c r="F47" s="28"/>
+        <v>331</v>
+      </c>
+      <c r="D47" s="26" t="s">
+        <v>23</v>
+      </c>
+      <c r="E47" s="0" t="s">
+        <v>350</v>
+      </c>
+      <c r="F47" s="28" t="s">
+        <v>251</v>
+      </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="28" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="B48" s="28" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="C48" s="28" t="s">
-        <v>326</v>
-      </c>
-      <c r="F48" s="28"/>
+        <v>331</v>
+      </c>
+      <c r="D48" s="26" t="s">
+        <v>23</v>
+      </c>
+      <c r="E48" s="0" t="s">
+        <v>352</v>
+      </c>
+      <c r="F48" s="28" t="s">
+        <v>251</v>
+      </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="28" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="B49" s="28" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="C49" s="28" t="s">
-        <v>326</v>
-      </c>
-      <c r="F49" s="28"/>
+        <v>331</v>
+      </c>
+      <c r="D49" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="E49" s="0" t="s">
+        <v>354</v>
+      </c>
+      <c r="F49" s="28" t="s">
+        <v>251</v>
+      </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="28" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="B50" s="28" t="s">
-        <v>355</v>
+        <v>349</v>
       </c>
       <c r="C50" s="28" t="s">
-        <v>275</v>
-      </c>
-      <c r="F50" s="28"/>
+        <v>331</v>
+      </c>
+      <c r="D50" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="E50" s="0" t="s">
+        <v>356</v>
+      </c>
+      <c r="F50" s="28" t="s">
+        <v>251</v>
+      </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="28" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="B51" s="28" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="C51" s="28" t="s">
-        <v>275</v>
-      </c>
-      <c r="F51" s="28"/>
+        <v>331</v>
+      </c>
+      <c r="D51" s="26" t="s">
+        <v>23</v>
+      </c>
+      <c r="E51" s="0" t="s">
+        <v>359</v>
+      </c>
+      <c r="F51" s="28" t="s">
+        <v>251</v>
+      </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="28" t="s">
+        <v>360</v>
+      </c>
+      <c r="B52" s="28" t="s">
         <v>358</v>
       </c>
-      <c r="B52" s="28" t="s">
-        <v>359</v>
-      </c>
       <c r="C52" s="28" t="s">
-        <v>275</v>
-      </c>
-      <c r="F52" s="28"/>
+        <v>331</v>
+      </c>
+      <c r="D52" s="26" t="s">
+        <v>23</v>
+      </c>
+      <c r="E52" s="0" t="s">
+        <v>361</v>
+      </c>
+      <c r="F52" s="28" t="s">
+        <v>251</v>
+      </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="28" t="s">
-        <v>360</v>
+        <v>362</v>
       </c>
       <c r="B53" s="28" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="C53" s="28" t="s">
-        <v>329</v>
-      </c>
-      <c r="F53" s="28"/>
+        <v>331</v>
+      </c>
+      <c r="D53" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="E53" s="0" t="s">
+        <v>363</v>
+      </c>
+      <c r="F53" s="28" t="s">
+        <v>251</v>
+      </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="28" t="s">
-        <v>362</v>
+        <v>364</v>
       </c>
       <c r="B54" s="28" t="s">
-        <v>363</v>
+        <v>358</v>
       </c>
       <c r="C54" s="28" t="s">
-        <v>326</v>
-      </c>
-      <c r="F54" s="28"/>
+        <v>331</v>
+      </c>
+      <c r="D54" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="E54" s="0" t="s">
+        <v>365</v>
+      </c>
+      <c r="F54" s="28" t="s">
+        <v>251</v>
+      </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="28" t="s">
-        <v>364</v>
+        <v>366</v>
       </c>
       <c r="B55" s="28" t="s">
-        <v>365</v>
+        <v>367</v>
       </c>
       <c r="C55" s="28" t="s">
-        <v>326</v>
-      </c>
-      <c r="F55" s="28"/>
+        <v>274</v>
+      </c>
+      <c r="F55" s="28" t="s">
+        <v>251</v>
+      </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="28" t="s">
-        <v>366</v>
+        <v>368</v>
       </c>
       <c r="B56" s="28" t="s">
-        <v>367</v>
+        <v>369</v>
       </c>
       <c r="C56" s="28" t="s">
-        <v>326</v>
-      </c>
-      <c r="F56" s="28"/>
+        <v>331</v>
+      </c>
+      <c r="F56" s="28" t="s">
+        <v>251</v>
+      </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="28" t="s">
-        <v>368</v>
+        <v>370</v>
       </c>
       <c r="B57" s="28" t="s">
-        <v>369</v>
+        <v>371</v>
       </c>
       <c r="C57" s="28" t="s">
-        <v>326</v>
+        <v>331</v>
       </c>
       <c r="F57" s="28"/>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="28" t="s">
-        <v>29</v>
+        <v>372</v>
       </c>
       <c r="B58" s="28" t="s">
-        <v>370</v>
+        <v>373</v>
       </c>
       <c r="C58" s="28" t="s">
-        <v>329</v>
+        <v>331</v>
       </c>
       <c r="F58" s="28"/>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="28" t="s">
-        <v>371</v>
+        <v>374</v>
       </c>
       <c r="B59" s="28" t="s">
-        <v>372</v>
+        <v>375</v>
       </c>
       <c r="C59" s="28" t="s">
-        <v>326</v>
+        <v>331</v>
       </c>
       <c r="F59" s="28"/>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="28" t="s">
-        <v>240</v>
+        <v>376</v>
       </c>
       <c r="B60" s="28" t="s">
-        <v>373</v>
+        <v>377</v>
       </c>
       <c r="C60" s="28" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="F60" s="28"/>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="28" t="s">
-        <v>374</v>
+        <v>378</v>
       </c>
       <c r="B61" s="28" t="s">
-        <v>375</v>
+        <v>379</v>
       </c>
       <c r="C61" s="28" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="F61" s="28"/>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="28" t="s">
-        <v>376</v>
+        <v>380</v>
       </c>
       <c r="B62" s="28" t="s">
-        <v>377</v>
+        <v>381</v>
       </c>
       <c r="C62" s="28" t="s">
-        <v>275</v>
+        <v>325</v>
       </c>
       <c r="F62" s="28"/>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="28" t="s">
-        <v>378</v>
+        <v>382</v>
       </c>
       <c r="B63" s="28" t="s">
-        <v>379</v>
+        <v>383</v>
       </c>
       <c r="C63" s="28" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="F63" s="28"/>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="28" t="s">
-        <v>380</v>
+        <v>384</v>
       </c>
       <c r="B64" s="28" t="s">
-        <v>381</v>
+        <v>385</v>
       </c>
       <c r="C64" s="28" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="F64" s="28"/>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="28" t="s">
-        <v>382</v>
+        <v>386</v>
       </c>
       <c r="B65" s="28" t="s">
-        <v>383</v>
+        <v>387</v>
       </c>
       <c r="C65" s="28" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="F65" s="28"/>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="28" t="s">
-        <v>384</v>
+        <v>388</v>
       </c>
       <c r="B66" s="28" t="s">
-        <v>385</v>
+        <v>389</v>
       </c>
       <c r="C66" s="28" t="s">
-        <v>275</v>
+        <v>331</v>
       </c>
       <c r="F66" s="28"/>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="28" t="s">
-        <v>386</v>
+        <v>390</v>
       </c>
       <c r="B67" s="28" t="s">
-        <v>387</v>
+        <v>391</v>
       </c>
       <c r="C67" s="28" t="s">
-        <v>275</v>
+        <v>325</v>
       </c>
       <c r="F67" s="28"/>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="28" t="s">
-        <v>388</v>
+        <v>392</v>
       </c>
       <c r="B68" s="28" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
       <c r="C68" s="28" t="s">
-        <v>275</v>
+        <v>325</v>
       </c>
       <c r="F68" s="28"/>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="28" t="s">
-        <v>390</v>
+        <v>394</v>
       </c>
       <c r="B69" s="28" t="s">
-        <v>391</v>
+        <v>395</v>
       </c>
       <c r="C69" s="28" t="s">
-        <v>275</v>
+        <v>325</v>
       </c>
       <c r="F69" s="28"/>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="28" t="s">
-        <v>392</v>
+        <v>396</v>
       </c>
       <c r="B70" s="28" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
       <c r="C70" s="28" t="s">
-        <v>248</v>
+        <v>325</v>
       </c>
       <c r="F70" s="28"/>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="28" t="s">
-        <v>394</v>
+        <v>29</v>
       </c>
       <c r="B71" s="28" t="s">
-        <v>395</v>
+        <v>398</v>
       </c>
       <c r="C71" s="28" t="s">
-        <v>396</v>
+        <v>331</v>
       </c>
       <c r="F71" s="28"/>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="28" t="s">
-        <v>397</v>
+        <v>399</v>
       </c>
       <c r="B72" s="28" t="s">
-        <v>398</v>
+        <v>400</v>
       </c>
       <c r="C72" s="28" t="s">
-        <v>396</v>
+        <v>325</v>
       </c>
       <c r="F72" s="28"/>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="28" t="s">
-        <v>399</v>
+        <v>240</v>
       </c>
       <c r="B73" s="28" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="C73" s="28" t="s">
-        <v>396</v>
+        <v>325</v>
       </c>
       <c r="F73" s="28"/>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="28" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="B74" s="28" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="C74" s="28" t="s">
-        <v>396</v>
+        <v>331</v>
       </c>
       <c r="F74" s="28"/>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="28" t="s">
-        <v>195</v>
+        <v>404</v>
       </c>
       <c r="B75" s="28" t="s">
-        <v>403</v>
+        <v>405</v>
       </c>
       <c r="C75" s="28" t="s">
-        <v>404</v>
+        <v>274</v>
       </c>
       <c r="F75" s="28"/>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="28" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="B76" s="28" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="C76" s="28" t="s">
-        <v>404</v>
+        <v>274</v>
       </c>
       <c r="F76" s="28"/>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="28" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="B77" s="28" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="C77" s="28" t="s">
-        <v>404</v>
+        <v>274</v>
       </c>
       <c r="F77" s="28"/>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="28" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="B78" s="28" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="C78" s="28" t="s">
-        <v>404</v>
+        <v>274</v>
       </c>
       <c r="F78" s="28"/>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="28" t="s">
-        <v>194</v>
+        <v>412</v>
       </c>
       <c r="B79" s="28" t="s">
-        <v>411</v>
+        <v>413</v>
       </c>
       <c r="C79" s="28" t="s">
-        <v>404</v>
+        <v>274</v>
       </c>
       <c r="F79" s="28"/>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="28" t="s">
-        <v>412</v>
+        <v>414</v>
       </c>
       <c r="B80" s="28" t="s">
-        <v>413</v>
+        <v>415</v>
       </c>
       <c r="C80" s="28" t="s">
-        <v>396</v>
+        <v>274</v>
       </c>
       <c r="F80" s="28"/>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="28" t="s">
-        <v>414</v>
+        <v>416</v>
       </c>
       <c r="B81" s="28" t="s">
-        <v>415</v>
+        <v>417</v>
       </c>
       <c r="C81" s="28" t="s">
-        <v>396</v>
+        <v>274</v>
       </c>
       <c r="F81" s="28"/>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="28" t="s">
-        <v>416</v>
+        <v>418</v>
       </c>
       <c r="B82" s="28" t="s">
-        <v>417</v>
+        <v>419</v>
       </c>
       <c r="C82" s="28" t="s">
-        <v>396</v>
+        <v>274</v>
       </c>
       <c r="F82" s="28"/>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="28" t="s">
-        <v>418</v>
+        <v>420</v>
       </c>
       <c r="B83" s="28" t="s">
-        <v>419</v>
+        <v>421</v>
       </c>
       <c r="C83" s="28" t="s">
-        <v>326</v>
+        <v>248</v>
       </c>
       <c r="F83" s="28"/>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="28" t="s">
-        <v>420</v>
+        <v>422</v>
       </c>
       <c r="B84" s="28" t="s">
-        <v>421</v>
+        <v>423</v>
       </c>
       <c r="C84" s="28" t="s">
-        <v>329</v>
+        <v>424</v>
       </c>
       <c r="F84" s="28"/>
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="28" t="s">
-        <v>422</v>
+        <v>425</v>
       </c>
       <c r="B85" s="28" t="s">
-        <v>423</v>
+        <v>426</v>
       </c>
       <c r="C85" s="28" t="s">
-        <v>275</v>
+        <v>424</v>
       </c>
       <c r="F85" s="28"/>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="28" t="s">
+        <v>427</v>
+      </c>
+      <c r="B86" s="28" t="s">
+        <v>428</v>
+      </c>
+      <c r="C86" s="28" t="s">
         <v>424</v>
-      </c>
-      <c r="B86" s="28" t="s">
-        <v>425</v>
-      </c>
-      <c r="C86" s="28" t="s">
-        <v>275</v>
       </c>
       <c r="F86" s="28"/>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="28" t="s">
-        <v>426</v>
+        <v>429</v>
       </c>
       <c r="B87" s="28" t="s">
-        <v>427</v>
+        <v>430</v>
       </c>
       <c r="C87" s="28" t="s">
-        <v>329</v>
+        <v>424</v>
       </c>
       <c r="F87" s="28"/>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="28" t="s">
-        <v>428</v>
+        <v>195</v>
       </c>
       <c r="B88" s="28" t="s">
-        <v>429</v>
+        <v>431</v>
       </c>
       <c r="C88" s="28" t="s">
-        <v>329</v>
+        <v>432</v>
       </c>
       <c r="F88" s="28"/>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="28" t="s">
-        <v>430</v>
+        <v>433</v>
       </c>
       <c r="B89" s="28" t="s">
-        <v>431</v>
+        <v>434</v>
       </c>
       <c r="C89" s="28" t="s">
-        <v>329</v>
+        <v>432</v>
       </c>
       <c r="F89" s="28"/>
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="28" t="s">
+        <v>435</v>
+      </c>
+      <c r="B90" s="28" t="s">
+        <v>436</v>
+      </c>
+      <c r="C90" s="28" t="s">
         <v>432</v>
-      </c>
-      <c r="B90" s="28" t="s">
-        <v>433</v>
-      </c>
-      <c r="C90" s="28" t="s">
-        <v>329</v>
       </c>
       <c r="F90" s="28"/>
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="28" t="s">
-        <v>434</v>
+        <v>437</v>
       </c>
       <c r="B91" s="28" t="s">
-        <v>435</v>
+        <v>438</v>
       </c>
       <c r="C91" s="28" t="s">
-        <v>326</v>
+        <v>432</v>
       </c>
       <c r="F91" s="28"/>
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="28" t="s">
-        <v>436</v>
+        <v>194</v>
       </c>
       <c r="B92" s="28" t="s">
-        <v>437</v>
+        <v>439</v>
       </c>
       <c r="C92" s="28" t="s">
-        <v>326</v>
+        <v>432</v>
       </c>
       <c r="F92" s="28"/>
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="28" t="s">
-        <v>438</v>
+        <v>440</v>
       </c>
       <c r="B93" s="28" t="s">
-        <v>439</v>
+        <v>441</v>
       </c>
       <c r="C93" s="28" t="s">
-        <v>326</v>
+        <v>424</v>
       </c>
       <c r="F93" s="28"/>
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="28" t="s">
-        <v>440</v>
+        <v>442</v>
       </c>
       <c r="B94" s="28" t="s">
-        <v>441</v>
+        <v>443</v>
       </c>
       <c r="C94" s="28" t="s">
-        <v>326</v>
+        <v>424</v>
       </c>
       <c r="F94" s="28"/>
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="28" t="s">
-        <v>442</v>
+        <v>444</v>
       </c>
       <c r="B95" s="28" t="s">
-        <v>443</v>
+        <v>445</v>
       </c>
       <c r="C95" s="28" t="s">
-        <v>329</v>
+        <v>424</v>
       </c>
       <c r="F95" s="28"/>
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="28" t="s">
-        <v>444</v>
+        <v>446</v>
       </c>
       <c r="B96" s="28" t="s">
-        <v>445</v>
+        <v>447</v>
       </c>
       <c r="C96" s="28" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="F96" s="28"/>
     </row>
     <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="28" t="s">
-        <v>446</v>
+        <v>448</v>
       </c>
       <c r="B97" s="28" t="s">
-        <v>447</v>
+        <v>449</v>
       </c>
       <c r="C97" s="28" t="s">
-        <v>326</v>
+        <v>331</v>
       </c>
       <c r="F97" s="28"/>
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="28" t="s">
-        <v>448</v>
+        <v>450</v>
       </c>
       <c r="B98" s="28" t="s">
-        <v>449</v>
+        <v>451</v>
       </c>
       <c r="C98" s="28" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="F98" s="28"/>
     </row>
     <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="28" t="s">
-        <v>450</v>
+        <v>452</v>
       </c>
       <c r="B99" s="28" t="s">
-        <v>451</v>
+        <v>453</v>
       </c>
       <c r="C99" s="28" t="s">
-        <v>329</v>
+        <v>274</v>
       </c>
       <c r="F99" s="28"/>
     </row>
     <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="28" t="s">
-        <v>452</v>
+        <v>454</v>
       </c>
       <c r="B100" s="28" t="s">
-        <v>453</v>
+        <v>455</v>
       </c>
       <c r="C100" s="28" t="s">
-        <v>326</v>
+        <v>331</v>
       </c>
       <c r="F100" s="28"/>
     </row>
     <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="28" t="s">
-        <v>454</v>
+        <v>456</v>
       </c>
       <c r="B101" s="28" t="s">
-        <v>455</v>
+        <v>457</v>
       </c>
       <c r="C101" s="28" t="s">
-        <v>329</v>
+        <v>331</v>
       </c>
       <c r="F101" s="28"/>
     </row>
     <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="28" t="s">
-        <v>456</v>
+        <v>458</v>
       </c>
       <c r="B102" s="28" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
       <c r="C102" s="28" t="s">
-        <v>275</v>
+        <v>331</v>
       </c>
       <c r="F102" s="28"/>
     </row>
     <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="28" t="s">
-        <v>458</v>
+        <v>460</v>
       </c>
       <c r="B103" s="28" t="s">
-        <v>459</v>
+        <v>461</v>
       </c>
       <c r="C103" s="28" t="s">
-        <v>326</v>
+        <v>331</v>
       </c>
       <c r="F103" s="28"/>
     </row>
     <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="28" t="s">
-        <v>460</v>
+        <v>462</v>
       </c>
       <c r="B104" s="28" t="s">
-        <v>461</v>
+        <v>463</v>
       </c>
       <c r="C104" s="28" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="F104" s="28"/>
     </row>
     <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="28" t="s">
-        <v>462</v>
+        <v>464</v>
       </c>
       <c r="B105" s="28" t="s">
-        <v>463</v>
+        <v>465</v>
       </c>
       <c r="C105" s="28" t="s">
-        <v>396</v>
+        <v>325</v>
       </c>
       <c r="F105" s="28"/>
     </row>
     <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="28" t="s">
-        <v>464</v>
+        <v>466</v>
       </c>
       <c r="B106" s="28" t="s">
-        <v>464</v>
+        <v>467</v>
       </c>
       <c r="C106" s="28" t="s">
-        <v>291</v>
+        <v>325</v>
       </c>
       <c r="F106" s="28"/>
     </row>
     <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="28" t="s">
-        <v>465</v>
+        <v>468</v>
       </c>
       <c r="B107" s="28" t="s">
-        <v>466</v>
+        <v>469</v>
       </c>
       <c r="C107" s="28" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="F107" s="28"/>
     </row>
     <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="28" t="s">
-        <v>467</v>
+        <v>470</v>
       </c>
       <c r="B108" s="28" t="s">
-        <v>468</v>
+        <v>471</v>
       </c>
       <c r="C108" s="28" t="s">
-        <v>275</v>
+        <v>331</v>
       </c>
       <c r="F108" s="28"/>
     </row>
     <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="28" t="s">
-        <v>469</v>
+        <v>472</v>
       </c>
       <c r="B109" s="28" t="s">
-        <v>470</v>
+        <v>473</v>
       </c>
       <c r="C109" s="28" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="F109" s="28"/>
     </row>
     <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="28" t="s">
-        <v>471</v>
+        <v>474</v>
       </c>
       <c r="B110" s="28" t="s">
-        <v>472</v>
+        <v>475</v>
       </c>
       <c r="C110" s="28" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="F110" s="28"/>
     </row>
     <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="28" t="s">
-        <v>473</v>
+        <v>476</v>
       </c>
       <c r="B111" s="28" t="s">
-        <v>474</v>
+        <v>477</v>
       </c>
       <c r="C111" s="28" t="s">
-        <v>248</v>
+        <v>274</v>
       </c>
       <c r="F111" s="28"/>
     </row>
     <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="28" t="s">
-        <v>475</v>
+        <v>478</v>
       </c>
       <c r="B112" s="28" t="s">
-        <v>476</v>
+        <v>479</v>
       </c>
       <c r="C112" s="28" t="s">
-        <v>329</v>
+        <v>331</v>
       </c>
       <c r="F112" s="28"/>
     </row>
     <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="28" t="s">
-        <v>477</v>
+        <v>480</v>
       </c>
       <c r="B113" s="28" t="s">
-        <v>478</v>
+        <v>481</v>
       </c>
       <c r="C113" s="28" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="F113" s="28"/>
     </row>
     <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="28" t="s">
-        <v>479</v>
+        <v>482</v>
       </c>
       <c r="B114" s="28" t="s">
-        <v>480</v>
+        <v>483</v>
       </c>
       <c r="C114" s="28" t="s">
-        <v>329</v>
+        <v>331</v>
       </c>
       <c r="F114" s="28"/>
     </row>
     <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="28" t="s">
-        <v>481</v>
+        <v>484</v>
       </c>
       <c r="B115" s="28" t="s">
-        <v>482</v>
+        <v>485</v>
       </c>
       <c r="C115" s="28" t="s">
-        <v>329</v>
+        <v>274</v>
       </c>
       <c r="F115" s="28"/>
     </row>
     <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="28" t="s">
-        <v>237</v>
+        <v>486</v>
       </c>
       <c r="B116" s="28" t="s">
-        <v>483</v>
+        <v>487</v>
       </c>
       <c r="C116" s="28" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="F116" s="28"/>
     </row>
     <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="28" t="s">
-        <v>484</v>
+        <v>488</v>
       </c>
       <c r="B117" s="28" t="s">
-        <v>485</v>
+        <v>489</v>
       </c>
       <c r="C117" s="28" t="s">
-        <v>329</v>
+        <v>331</v>
       </c>
       <c r="F117" s="28"/>
     </row>
     <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="28" t="s">
-        <v>486</v>
+        <v>490</v>
       </c>
       <c r="B118" s="28" t="s">
-        <v>487</v>
+        <v>491</v>
       </c>
       <c r="C118" s="28" t="s">
-        <v>248</v>
+        <v>424</v>
       </c>
       <c r="F118" s="28"/>
     </row>
     <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="28" t="s">
-        <v>168</v>
+        <v>492</v>
       </c>
       <c r="B119" s="28" t="s">
-        <v>488</v>
+        <v>492</v>
       </c>
       <c r="C119" s="28" t="s">
-        <v>248</v>
+        <v>290</v>
       </c>
       <c r="F119" s="28"/>
     </row>
     <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="28" t="s">
-        <v>489</v>
+        <v>493</v>
       </c>
       <c r="B120" s="28" t="s">
-        <v>490</v>
+        <v>494</v>
       </c>
       <c r="C120" s="28" t="s">
-        <v>248</v>
+        <v>325</v>
       </c>
       <c r="F120" s="28"/>
     </row>
     <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="28" t="s">
-        <v>238</v>
+        <v>495</v>
       </c>
       <c r="B121" s="28" t="s">
-        <v>491</v>
+        <v>496</v>
       </c>
       <c r="C121" s="28" t="s">
-        <v>326</v>
+        <v>274</v>
       </c>
       <c r="F121" s="28"/>
     </row>
     <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="28" t="s">
-        <v>217</v>
+        <v>497</v>
       </c>
       <c r="B122" s="28" t="s">
-        <v>492</v>
+        <v>498</v>
       </c>
       <c r="C122" s="28" t="s">
-        <v>275</v>
+        <v>325</v>
       </c>
       <c r="F122" s="28"/>
     </row>
     <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="28" t="s">
-        <v>493</v>
+        <v>499</v>
       </c>
       <c r="B123" s="28" t="s">
-        <v>494</v>
+        <v>500</v>
       </c>
       <c r="C123" s="28" t="s">
-        <v>326</v>
+        <v>331</v>
       </c>
       <c r="F123" s="28"/>
+    </row>
+    <row r="124" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A124" s="28" t="s">
+        <v>501</v>
+      </c>
+      <c r="B124" s="28" t="s">
+        <v>502</v>
+      </c>
+      <c r="C124" s="28" t="s">
+        <v>248</v>
+      </c>
+      <c r="F124" s="28"/>
+    </row>
+    <row r="125" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A125" s="28" t="s">
+        <v>503</v>
+      </c>
+      <c r="B125" s="28" t="s">
+        <v>504</v>
+      </c>
+      <c r="C125" s="28" t="s">
+        <v>331</v>
+      </c>
+      <c r="F125" s="28"/>
+    </row>
+    <row r="126" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A126" s="28" t="s">
+        <v>505</v>
+      </c>
+      <c r="B126" s="28" t="s">
+        <v>506</v>
+      </c>
+      <c r="C126" s="28" t="s">
+        <v>331</v>
+      </c>
+      <c r="F126" s="28"/>
+    </row>
+    <row r="127" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A127" s="28" t="s">
+        <v>507</v>
+      </c>
+      <c r="B127" s="28" t="s">
+        <v>508</v>
+      </c>
+      <c r="C127" s="28" t="s">
+        <v>331</v>
+      </c>
+      <c r="F127" s="28"/>
+    </row>
+    <row r="128" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A128" s="28" t="s">
+        <v>509</v>
+      </c>
+      <c r="B128" s="28" t="s">
+        <v>510</v>
+      </c>
+      <c r="C128" s="28" t="s">
+        <v>331</v>
+      </c>
+      <c r="F128" s="28"/>
+    </row>
+    <row r="129" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A129" s="28" t="s">
+        <v>237</v>
+      </c>
+      <c r="B129" s="28" t="s">
+        <v>511</v>
+      </c>
+      <c r="C129" s="28" t="s">
+        <v>325</v>
+      </c>
+      <c r="F129" s="28"/>
+    </row>
+    <row r="130" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A130" s="28" t="s">
+        <v>512</v>
+      </c>
+      <c r="B130" s="28" t="s">
+        <v>513</v>
+      </c>
+      <c r="C130" s="28" t="s">
+        <v>331</v>
+      </c>
+      <c r="F130" s="28"/>
+    </row>
+    <row r="131" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A131" s="28" t="s">
+        <v>514</v>
+      </c>
+      <c r="B131" s="28" t="s">
+        <v>515</v>
+      </c>
+      <c r="C131" s="28" t="s">
+        <v>248</v>
+      </c>
+      <c r="F131" s="28"/>
+    </row>
+    <row r="132" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A132" s="28" t="s">
+        <v>168</v>
+      </c>
+      <c r="B132" s="28" t="s">
+        <v>516</v>
+      </c>
+      <c r="C132" s="28" t="s">
+        <v>248</v>
+      </c>
+      <c r="F132" s="28"/>
+    </row>
+    <row r="133" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A133" s="28" t="s">
+        <v>517</v>
+      </c>
+      <c r="B133" s="28" t="s">
+        <v>518</v>
+      </c>
+      <c r="C133" s="28" t="s">
+        <v>248</v>
+      </c>
+      <c r="F133" s="28"/>
+    </row>
+    <row r="134" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A134" s="28" t="s">
+        <v>238</v>
+      </c>
+      <c r="B134" s="28" t="s">
+        <v>519</v>
+      </c>
+      <c r="C134" s="28" t="s">
+        <v>325</v>
+      </c>
+      <c r="F134" s="28"/>
+    </row>
+    <row r="135" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A135" s="28" t="s">
+        <v>217</v>
+      </c>
+      <c r="B135" s="28" t="s">
+        <v>520</v>
+      </c>
+      <c r="C135" s="28" t="s">
+        <v>274</v>
+      </c>
+      <c r="F135" s="28"/>
+    </row>
+    <row r="136" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A136" s="28" t="s">
+        <v>521</v>
+      </c>
+      <c r="B136" s="28" t="s">
+        <v>522</v>
+      </c>
+      <c r="C136" s="28" t="s">
+        <v>325</v>
+      </c>
+      <c r="F136" s="28"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
La till flera kontrakt till dokument
</commit_message>
<xml_diff>
--- a/manuell_berakning_minimum_kapital.xlsx
+++ b/manuell_berakning_minimum_kapital.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="907" uniqueCount="523">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1057" uniqueCount="572">
   <si>
     <t xml:space="preserve">Namn</t>
   </si>
@@ -1122,22 +1122,46 @@
     <t xml:space="preserve">IX.D.NASDAQ.FWM1.IP</t>
   </si>
   <si>
-    <t xml:space="preserve">KC HRW Wheat</t>
+    <t xml:space="preserve">KC HRW Wheat 50€</t>
   </si>
   <si>
     <t xml:space="preserve">KE</t>
   </si>
   <si>
+    <t xml:space="preserve">TecDAX 2€ mini</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FTDX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TM.D.TECDAX.IFM.IP</t>
+  </si>
+  <si>
     <t xml:space="preserve">TecDAX</t>
   </si>
   <si>
-    <t xml:space="preserve">FTDX</t>
+    <t xml:space="preserve">TM.D.TECDAX.IFD.IP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Swiss Market Index 10CHF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FSMI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IX.D.SMI.IFD.IP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Swiss Market Index 2CHF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IX.D.SMI.IFM.IP</t>
   </si>
   <si>
     <t xml:space="preserve">Swiss Market Index</t>
   </si>
   <si>
-    <t xml:space="preserve">FSMI</t>
+    <t xml:space="preserve">IX.D.SMI.FWM2.IP</t>
   </si>
   <si>
     <t xml:space="preserve">E-mini S&amp;P MidCap 400</t>
@@ -1146,64 +1170,283 @@
     <t xml:space="preserve">EMD</t>
   </si>
   <si>
+    <t xml:space="preserve">Nikkei 225 Dollar 5$</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NKD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IX.D.NIKKEI.IFD.IP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nikkei 225 Dollar 1$</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IX.D.NIKKEI.IFM.IP</t>
+  </si>
+  <si>
     <t xml:space="preserve">Nikkei 225 Dollar</t>
   </si>
   <si>
-    <t xml:space="preserve">NKD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5-Year U.S. T-Note</t>
+    <t xml:space="preserve">IX.D.NIKFUT.FWM1.IP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5-Year U.S. T-Note 2$</t>
   </si>
   <si>
     <t xml:space="preserve">ZF</t>
   </si>
   <si>
-    <t xml:space="preserve">U.S. T-Bond</t>
+    <t xml:space="preserve">IR.D.05YEAR100.FWM2.IP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5-Year U.S. T-Note 10$</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IR.D.05YEAR100.FWS2.IP</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">U.S. T-Bond </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">2$</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">ZB</t>
   </si>
   <si>
-    <t xml:space="preserve">2-Year U.S. T-Note</t>
+    <t xml:space="preserve">IR.D.BOND100.FWS.IP</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">U.S. T-Bond </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">10$</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">IR.D.BOND100.FWM.IP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2-Year U.S. T-Note 2$</t>
   </si>
   <si>
     <t xml:space="preserve">ZT</t>
   </si>
   <si>
-    <t xml:space="preserve">Oats</t>
+    <t xml:space="preserve">IR.D.02YEAR100.FWM2.IP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2-Year U.S. T-Note 10$</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IR.D.02YEAR100.FWS2.IP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Oats 25$</t>
   </si>
   <si>
     <t xml:space="preserve">ZO</t>
   </si>
   <si>
-    <t xml:space="preserve">Chicago SRW Wheat</t>
+    <t xml:space="preserve">CO.D.O.FWM2.IP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Oats 50$</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CO.D.O.FWS2.IP</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Chicago SRW Wheat </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">50€</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">ZW</t>
   </si>
   <si>
-    <t xml:space="preserve">Soybean</t>
+    <t xml:space="preserve">CC.D.W.UNC.IP</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Chicago SRW Wheat </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">1€</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">CC.D.W.UME.IP</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Chicago SRW Wheat </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">25$</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">CO.D.W.FWM1.IP</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Chicago SRW Wheat </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">50$</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">CO.D.W.FWS1.IP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Soybean 50$</t>
   </si>
   <si>
     <t xml:space="preserve">ZS</t>
   </si>
   <si>
-    <t xml:space="preserve">DAX</t>
+    <t xml:space="preserve">CC.D.S.UNC.IP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Soybean 1€</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CC.D.S.UME.IP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CO.D.S.FWS2.IP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Soybean 25$</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CO.D.S.FWM2.IP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DAX 1€</t>
   </si>
   <si>
     <t xml:space="preserve">FDAX</t>
   </si>
   <si>
-    <t xml:space="preserve">Euro-Bund</t>
+    <t xml:space="preserve">IX.D.DAX.INE.IP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DAX 25€</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IX.D.DAX.FWS1.IP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DAX 5€</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IX.D.DAX.FWM1.IP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Euro-Bund 10€</t>
   </si>
   <si>
     <t xml:space="preserve">FGBL</t>
   </si>
   <si>
-    <t xml:space="preserve">Euro-Schatz</t>
+    <t xml:space="preserve">IR.D.FGBL.FWJ2.IP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Euro-Bund 2€</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IR.D.FGBL.FWM2.IP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Euro-Schatz 2€</t>
   </si>
   <si>
     <t xml:space="preserve">FGBS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IR.D.FGBS.FWM2.IP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Euro-Schatz 10€</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IR.D.FGBS.FWS2.IP</t>
   </si>
   <si>
     <t xml:space="preserve">Euro-Bobl</t>
@@ -1606,7 +1849,7 @@
     <numFmt numFmtId="169" formatCode="[$$-409]#,##0.0;[RED]\-[$$-409]#,##0.0"/>
     <numFmt numFmtId="170" formatCode="#,##0.00\ [$€-81D];[RED]\-#,##0.00\ [$€-81D]"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1653,6 +1896,11 @@
       <sz val="10"/>
       <name val="Liberation Mono;Courier New;DejaVu Sans Mono"/>
       <family val="3"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -1703,7 +1951,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1821,6 +2069,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -5204,10 +5456,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G136"/>
+  <dimension ref="A1:G155"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A46" activeCellId="0" sqref="A46"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A64" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E89" activeCellId="0" sqref="E89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5215,8 +5467,8 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="26" width="36.91"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="26" width="7.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="26" width="20.35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="26" width="20.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="22.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="26" width="7.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="23.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="26" width="22.58"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="14.09"/>
   </cols>
@@ -6264,7 +6516,7 @@
         <v>274</v>
       </c>
       <c r="F55" s="28" t="s">
-        <v>251</v>
+        <v>259</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6277,508 +6529,756 @@
       <c r="C56" s="28" t="s">
         <v>331</v>
       </c>
+      <c r="D56" s="26" t="s">
+        <v>23</v>
+      </c>
+      <c r="E56" s="0" t="s">
+        <v>370</v>
+      </c>
       <c r="F56" s="28" t="s">
         <v>251</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="28" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="B57" s="28" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="C57" s="28" t="s">
         <v>331</v>
       </c>
-      <c r="F57" s="28"/>
+      <c r="D57" s="26" t="s">
+        <v>23</v>
+      </c>
+      <c r="E57" s="0" t="s">
+        <v>372</v>
+      </c>
+      <c r="F57" s="28" t="s">
+        <v>251</v>
+      </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="28" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="B58" s="28" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="C58" s="28" t="s">
         <v>331</v>
       </c>
-      <c r="F58" s="28"/>
+      <c r="D58" s="26" t="s">
+        <v>23</v>
+      </c>
+      <c r="E58" s="0" t="s">
+        <v>375</v>
+      </c>
+      <c r="F58" s="28" t="s">
+        <v>251</v>
+      </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="28" t="s">
+        <v>376</v>
+      </c>
+      <c r="B59" s="28" t="s">
         <v>374</v>
-      </c>
-      <c r="B59" s="28" t="s">
-        <v>375</v>
       </c>
       <c r="C59" s="28" t="s">
         <v>331</v>
       </c>
-      <c r="F59" s="28"/>
+      <c r="D59" s="26" t="s">
+        <v>23</v>
+      </c>
+      <c r="E59" s="0" t="s">
+        <v>377</v>
+      </c>
+      <c r="F59" s="28" t="s">
+        <v>251</v>
+      </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="28" t="s">
-        <v>376</v>
+        <v>378</v>
       </c>
       <c r="B60" s="28" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="C60" s="28" t="s">
-        <v>325</v>
-      </c>
-      <c r="F60" s="28"/>
+        <v>331</v>
+      </c>
+      <c r="D60" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="E60" s="0" t="s">
+        <v>379</v>
+      </c>
+      <c r="F60" s="28" t="s">
+        <v>251</v>
+      </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="28" t="s">
-        <v>378</v>
+        <v>380</v>
       </c>
       <c r="B61" s="28" t="s">
-        <v>379</v>
+        <v>381</v>
       </c>
       <c r="C61" s="28" t="s">
-        <v>325</v>
-      </c>
-      <c r="F61" s="28"/>
+        <v>331</v>
+      </c>
+      <c r="F61" s="28" t="s">
+        <v>259</v>
+      </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="28" t="s">
-        <v>380</v>
+        <v>382</v>
       </c>
       <c r="B62" s="28" t="s">
-        <v>381</v>
+        <v>383</v>
       </c>
       <c r="C62" s="28" t="s">
-        <v>325</v>
-      </c>
-      <c r="F62" s="28"/>
+        <v>331</v>
+      </c>
+      <c r="D62" s="26" t="s">
+        <v>23</v>
+      </c>
+      <c r="E62" s="0" t="s">
+        <v>384</v>
+      </c>
+      <c r="F62" s="28" t="s">
+        <v>251</v>
+      </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="28" t="s">
-        <v>382</v>
+        <v>385</v>
       </c>
       <c r="B63" s="28" t="s">
         <v>383</v>
       </c>
       <c r="C63" s="28" t="s">
-        <v>274</v>
-      </c>
-      <c r="F63" s="28"/>
+        <v>331</v>
+      </c>
+      <c r="D63" s="26" t="s">
+        <v>23</v>
+      </c>
+      <c r="E63" s="0" t="s">
+        <v>386</v>
+      </c>
+      <c r="F63" s="28" t="s">
+        <v>251</v>
+      </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="28" t="s">
-        <v>384</v>
+        <v>387</v>
       </c>
       <c r="B64" s="28" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="C64" s="28" t="s">
-        <v>274</v>
-      </c>
-      <c r="F64" s="28"/>
+        <v>331</v>
+      </c>
+      <c r="D64" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="E64" s="0" t="s">
+        <v>388</v>
+      </c>
+      <c r="F64" s="28" t="s">
+        <v>251</v>
+      </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="28" t="s">
-        <v>386</v>
+        <v>389</v>
       </c>
       <c r="B65" s="28" t="s">
-        <v>387</v>
+        <v>390</v>
       </c>
       <c r="C65" s="28" t="s">
-        <v>274</v>
-      </c>
-      <c r="F65" s="28"/>
+        <v>325</v>
+      </c>
+      <c r="D65" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="E65" s="0" t="s">
+        <v>391</v>
+      </c>
+      <c r="F65" s="28" t="s">
+        <v>251</v>
+      </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="28" t="s">
-        <v>388</v>
+      <c r="A66" s="30" t="s">
+        <v>392</v>
       </c>
       <c r="B66" s="28" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="C66" s="28" t="s">
-        <v>331</v>
-      </c>
-      <c r="F66" s="28"/>
+        <v>325</v>
+      </c>
+      <c r="D66" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="E66" s="0" t="s">
+        <v>393</v>
+      </c>
+      <c r="F66" s="28" t="s">
+        <v>251</v>
+      </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="28" t="s">
-        <v>390</v>
+        <v>394</v>
       </c>
       <c r="B67" s="28" t="s">
-        <v>391</v>
+        <v>395</v>
       </c>
       <c r="C67" s="28" t="s">
         <v>325</v>
       </c>
-      <c r="F67" s="28"/>
+      <c r="D67" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="E67" s="0" t="s">
+        <v>396</v>
+      </c>
+      <c r="F67" s="28" t="s">
+        <v>251</v>
+      </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="28" t="s">
-        <v>392</v>
+        <v>397</v>
       </c>
       <c r="B68" s="28" t="s">
-        <v>393</v>
+        <v>395</v>
       </c>
       <c r="C68" s="28" t="s">
         <v>325</v>
       </c>
-      <c r="F68" s="28"/>
+      <c r="D68" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="E68" s="0" t="s">
+        <v>398</v>
+      </c>
+      <c r="F68" s="28" t="s">
+        <v>251</v>
+      </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="28" t="s">
-        <v>394</v>
+        <v>399</v>
       </c>
       <c r="B69" s="28" t="s">
-        <v>395</v>
+        <v>400</v>
       </c>
       <c r="C69" s="28" t="s">
         <v>325</v>
       </c>
-      <c r="F69" s="28"/>
+      <c r="D69" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="E69" s="0" t="s">
+        <v>401</v>
+      </c>
+      <c r="F69" s="28" t="s">
+        <v>251</v>
+      </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="28" t="s">
-        <v>396</v>
+        <v>402</v>
       </c>
       <c r="B70" s="28" t="s">
-        <v>397</v>
+        <v>400</v>
       </c>
       <c r="C70" s="28" t="s">
         <v>325</v>
       </c>
-      <c r="F70" s="28"/>
+      <c r="D70" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="E70" s="0" t="s">
+        <v>403</v>
+      </c>
+      <c r="F70" s="28" t="s">
+        <v>251</v>
+      </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="28" t="s">
-        <v>29</v>
+        <v>404</v>
       </c>
       <c r="B71" s="28" t="s">
-        <v>398</v>
+        <v>405</v>
       </c>
       <c r="C71" s="28" t="s">
-        <v>331</v>
-      </c>
-      <c r="F71" s="28"/>
+        <v>274</v>
+      </c>
+      <c r="D71" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="E71" s="0" t="s">
+        <v>406</v>
+      </c>
+      <c r="F71" s="28" t="s">
+        <v>251</v>
+      </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="28" t="s">
-        <v>399</v>
+        <v>407</v>
       </c>
       <c r="B72" s="28" t="s">
-        <v>400</v>
+        <v>405</v>
       </c>
       <c r="C72" s="28" t="s">
-        <v>325</v>
-      </c>
-      <c r="F72" s="28"/>
+        <v>274</v>
+      </c>
+      <c r="D72" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="E72" s="0" t="s">
+        <v>408</v>
+      </c>
+      <c r="F72" s="28" t="s">
+        <v>251</v>
+      </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="28" t="s">
-        <v>240</v>
+        <v>409</v>
       </c>
       <c r="B73" s="28" t="s">
-        <v>401</v>
+        <v>410</v>
       </c>
       <c r="C73" s="28" t="s">
-        <v>325</v>
-      </c>
-      <c r="F73" s="28"/>
+        <v>274</v>
+      </c>
+      <c r="D73" s="26" t="s">
+        <v>23</v>
+      </c>
+      <c r="E73" s="0" t="s">
+        <v>411</v>
+      </c>
+      <c r="F73" s="28" t="s">
+        <v>251</v>
+      </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="28" t="s">
-        <v>402</v>
+        <v>412</v>
       </c>
       <c r="B74" s="28" t="s">
-        <v>403</v>
+        <v>410</v>
       </c>
       <c r="C74" s="28" t="s">
-        <v>331</v>
-      </c>
-      <c r="F74" s="28"/>
+        <v>274</v>
+      </c>
+      <c r="D74" s="26" t="s">
+        <v>23</v>
+      </c>
+      <c r="E74" s="0" t="s">
+        <v>413</v>
+      </c>
+      <c r="F74" s="28" t="s">
+        <v>251</v>
+      </c>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="28" t="s">
-        <v>404</v>
+        <v>414</v>
       </c>
       <c r="B75" s="28" t="s">
-        <v>405</v>
+        <v>410</v>
       </c>
       <c r="C75" s="28" t="s">
         <v>274</v>
       </c>
-      <c r="F75" s="28"/>
+      <c r="D75" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="E75" s="0" t="s">
+        <v>415</v>
+      </c>
+      <c r="F75" s="28" t="s">
+        <v>251</v>
+      </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="28" t="s">
-        <v>406</v>
+        <v>416</v>
       </c>
       <c r="B76" s="28" t="s">
-        <v>407</v>
+        <v>410</v>
       </c>
       <c r="C76" s="28" t="s">
         <v>274</v>
       </c>
-      <c r="F76" s="28"/>
+      <c r="D76" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="E76" s="0" t="s">
+        <v>417</v>
+      </c>
+      <c r="F76" s="28" t="s">
+        <v>251</v>
+      </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="28" t="s">
-        <v>408</v>
+        <v>418</v>
       </c>
       <c r="B77" s="28" t="s">
-        <v>409</v>
+        <v>419</v>
       </c>
       <c r="C77" s="28" t="s">
         <v>274</v>
       </c>
-      <c r="F77" s="28"/>
+      <c r="D77" s="26" t="s">
+        <v>23</v>
+      </c>
+      <c r="E77" s="0" t="s">
+        <v>420</v>
+      </c>
+      <c r="F77" s="28" t="s">
+        <v>251</v>
+      </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="28" t="s">
-        <v>410</v>
+        <v>421</v>
       </c>
       <c r="B78" s="28" t="s">
-        <v>411</v>
+        <v>419</v>
       </c>
       <c r="C78" s="28" t="s">
         <v>274</v>
       </c>
-      <c r="F78" s="28"/>
+      <c r="D78" s="26" t="s">
+        <v>23</v>
+      </c>
+      <c r="E78" s="0" t="s">
+        <v>422</v>
+      </c>
+      <c r="F78" s="28" t="s">
+        <v>251</v>
+      </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="28" t="s">
-        <v>412</v>
+        <v>418</v>
       </c>
       <c r="B79" s="28" t="s">
-        <v>413</v>
+        <v>419</v>
       </c>
       <c r="C79" s="28" t="s">
         <v>274</v>
       </c>
-      <c r="F79" s="28"/>
+      <c r="D79" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="E79" s="0" t="s">
+        <v>423</v>
+      </c>
+      <c r="F79" s="28" t="s">
+        <v>251</v>
+      </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="28" t="s">
-        <v>414</v>
+        <v>424</v>
       </c>
       <c r="B80" s="28" t="s">
-        <v>415</v>
+        <v>419</v>
       </c>
       <c r="C80" s="28" t="s">
         <v>274</v>
       </c>
-      <c r="F80" s="28"/>
+      <c r="D80" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="E80" s="0" t="s">
+        <v>425</v>
+      </c>
+      <c r="F80" s="28" t="s">
+        <v>251</v>
+      </c>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="28" t="s">
-        <v>416</v>
+        <v>426</v>
       </c>
       <c r="B81" s="28" t="s">
-        <v>417</v>
+        <v>427</v>
       </c>
       <c r="C81" s="28" t="s">
-        <v>274</v>
-      </c>
-      <c r="F81" s="28"/>
+        <v>331</v>
+      </c>
+      <c r="D81" s="26" t="s">
+        <v>23</v>
+      </c>
+      <c r="E81" s="0" t="s">
+        <v>428</v>
+      </c>
+      <c r="F81" s="28" t="s">
+        <v>251</v>
+      </c>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="28" t="s">
-        <v>418</v>
+        <v>429</v>
       </c>
       <c r="B82" s="28" t="s">
-        <v>419</v>
+        <v>427</v>
       </c>
       <c r="C82" s="28" t="s">
-        <v>274</v>
-      </c>
-      <c r="F82" s="28"/>
+        <v>331</v>
+      </c>
+      <c r="D82" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="E82" s="0" t="s">
+        <v>430</v>
+      </c>
+      <c r="F82" s="28" t="s">
+        <v>251</v>
+      </c>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="28" t="s">
-        <v>420</v>
+        <v>431</v>
       </c>
       <c r="B83" s="28" t="s">
-        <v>421</v>
+        <v>427</v>
       </c>
       <c r="C83" s="28" t="s">
-        <v>248</v>
-      </c>
-      <c r="F83" s="28"/>
+        <v>331</v>
+      </c>
+      <c r="D83" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="E83" s="0" t="s">
+        <v>432</v>
+      </c>
+      <c r="F83" s="28" t="s">
+        <v>251</v>
+      </c>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="28" t="s">
-        <v>422</v>
+        <v>433</v>
       </c>
       <c r="B84" s="28" t="s">
-        <v>423</v>
+        <v>434</v>
       </c>
       <c r="C84" s="28" t="s">
-        <v>424</v>
-      </c>
-      <c r="F84" s="28"/>
+        <v>325</v>
+      </c>
+      <c r="D84" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="E84" s="0" t="s">
+        <v>435</v>
+      </c>
+      <c r="F84" s="28" t="s">
+        <v>251</v>
+      </c>
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="28" t="s">
-        <v>425</v>
+        <v>436</v>
       </c>
       <c r="B85" s="28" t="s">
-        <v>426</v>
+        <v>434</v>
       </c>
       <c r="C85" s="28" t="s">
-        <v>424</v>
-      </c>
-      <c r="F85" s="28"/>
+        <v>325</v>
+      </c>
+      <c r="D85" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="E85" s="0" t="s">
+        <v>437</v>
+      </c>
+      <c r="F85" s="28" t="s">
+        <v>251</v>
+      </c>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="28" t="s">
-        <v>427</v>
+        <v>438</v>
       </c>
       <c r="B86" s="28" t="s">
-        <v>428</v>
+        <v>439</v>
       </c>
       <c r="C86" s="28" t="s">
-        <v>424</v>
-      </c>
-      <c r="F86" s="28"/>
+        <v>325</v>
+      </c>
+      <c r="D86" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="E86" s="0" t="s">
+        <v>440</v>
+      </c>
+      <c r="F86" s="28" t="s">
+        <v>251</v>
+      </c>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="28" t="s">
-        <v>429</v>
+        <v>441</v>
       </c>
       <c r="B87" s="28" t="s">
-        <v>430</v>
+        <v>439</v>
       </c>
       <c r="C87" s="28" t="s">
-        <v>424</v>
-      </c>
-      <c r="F87" s="28"/>
+        <v>325</v>
+      </c>
+      <c r="D87" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="E87" s="0" t="s">
+        <v>442</v>
+      </c>
+      <c r="F87" s="28" t="s">
+        <v>251</v>
+      </c>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="28" t="s">
-        <v>195</v>
+        <v>443</v>
       </c>
       <c r="B88" s="28" t="s">
-        <v>431</v>
+        <v>444</v>
       </c>
       <c r="C88" s="28" t="s">
-        <v>432</v>
+        <v>325</v>
       </c>
       <c r="F88" s="28"/>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="28" t="s">
-        <v>433</v>
+        <v>445</v>
       </c>
       <c r="B89" s="28" t="s">
-        <v>434</v>
+        <v>446</v>
       </c>
       <c r="C89" s="28" t="s">
-        <v>432</v>
+        <v>325</v>
       </c>
       <c r="F89" s="28"/>
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="28" t="s">
-        <v>435</v>
+        <v>29</v>
       </c>
       <c r="B90" s="28" t="s">
-        <v>436</v>
+        <v>447</v>
       </c>
       <c r="C90" s="28" t="s">
-        <v>432</v>
+        <v>331</v>
       </c>
       <c r="F90" s="28"/>
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="28" t="s">
-        <v>437</v>
+        <v>448</v>
       </c>
       <c r="B91" s="28" t="s">
-        <v>438</v>
+        <v>449</v>
       </c>
       <c r="C91" s="28" t="s">
-        <v>432</v>
+        <v>325</v>
       </c>
       <c r="F91" s="28"/>
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="28" t="s">
-        <v>194</v>
+        <v>240</v>
       </c>
       <c r="B92" s="28" t="s">
-        <v>439</v>
+        <v>450</v>
       </c>
       <c r="C92" s="28" t="s">
-        <v>432</v>
+        <v>325</v>
       </c>
       <c r="F92" s="28"/>
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="28" t="s">
-        <v>440</v>
+        <v>451</v>
       </c>
       <c r="B93" s="28" t="s">
-        <v>441</v>
+        <v>452</v>
       </c>
       <c r="C93" s="28" t="s">
-        <v>424</v>
+        <v>331</v>
       </c>
       <c r="F93" s="28"/>
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="28" t="s">
-        <v>442</v>
+        <v>453</v>
       </c>
       <c r="B94" s="28" t="s">
-        <v>443</v>
+        <v>454</v>
       </c>
       <c r="C94" s="28" t="s">
-        <v>424</v>
+        <v>274</v>
       </c>
       <c r="F94" s="28"/>
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="28" t="s">
-        <v>444</v>
+        <v>455</v>
       </c>
       <c r="B95" s="28" t="s">
-        <v>445</v>
+        <v>456</v>
       </c>
       <c r="C95" s="28" t="s">
-        <v>424</v>
+        <v>274</v>
       </c>
       <c r="F95" s="28"/>
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="28" t="s">
-        <v>446</v>
+        <v>457</v>
       </c>
       <c r="B96" s="28" t="s">
-        <v>447</v>
+        <v>458</v>
       </c>
       <c r="C96" s="28" t="s">
-        <v>325</v>
+        <v>274</v>
       </c>
       <c r="F96" s="28"/>
     </row>
     <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="28" t="s">
-        <v>448</v>
+        <v>459</v>
       </c>
       <c r="B97" s="28" t="s">
-        <v>449</v>
+        <v>460</v>
       </c>
       <c r="C97" s="28" t="s">
-        <v>331</v>
+        <v>274</v>
       </c>
       <c r="F97" s="28"/>
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="28" t="s">
-        <v>450</v>
+        <v>461</v>
       </c>
       <c r="B98" s="28" t="s">
-        <v>451</v>
+        <v>462</v>
       </c>
       <c r="C98" s="28" t="s">
         <v>274</v>
@@ -6787,10 +7287,10 @@
     </row>
     <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="28" t="s">
-        <v>452</v>
+        <v>463</v>
       </c>
       <c r="B99" s="28" t="s">
-        <v>453</v>
+        <v>464</v>
       </c>
       <c r="C99" s="28" t="s">
         <v>274</v>
@@ -6799,334 +7299,334 @@
     </row>
     <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="28" t="s">
-        <v>454</v>
+        <v>465</v>
       </c>
       <c r="B100" s="28" t="s">
-        <v>455</v>
+        <v>466</v>
       </c>
       <c r="C100" s="28" t="s">
-        <v>331</v>
+        <v>274</v>
       </c>
       <c r="F100" s="28"/>
     </row>
     <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="28" t="s">
-        <v>456</v>
+        <v>467</v>
       </c>
       <c r="B101" s="28" t="s">
-        <v>457</v>
+        <v>468</v>
       </c>
       <c r="C101" s="28" t="s">
-        <v>331</v>
+        <v>274</v>
       </c>
       <c r="F101" s="28"/>
     </row>
     <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="28" t="s">
-        <v>458</v>
+        <v>469</v>
       </c>
       <c r="B102" s="28" t="s">
-        <v>459</v>
+        <v>470</v>
       </c>
       <c r="C102" s="28" t="s">
-        <v>331</v>
+        <v>248</v>
       </c>
       <c r="F102" s="28"/>
     </row>
     <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="28" t="s">
-        <v>460</v>
+        <v>471</v>
       </c>
       <c r="B103" s="28" t="s">
-        <v>461</v>
+        <v>472</v>
       </c>
       <c r="C103" s="28" t="s">
-        <v>331</v>
+        <v>473</v>
       </c>
       <c r="F103" s="28"/>
     </row>
     <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="28" t="s">
-        <v>462</v>
+        <v>474</v>
       </c>
       <c r="B104" s="28" t="s">
-        <v>463</v>
+        <v>475</v>
       </c>
       <c r="C104" s="28" t="s">
-        <v>325</v>
+        <v>473</v>
       </c>
       <c r="F104" s="28"/>
     </row>
     <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="28" t="s">
-        <v>464</v>
+        <v>476</v>
       </c>
       <c r="B105" s="28" t="s">
-        <v>465</v>
+        <v>477</v>
       </c>
       <c r="C105" s="28" t="s">
-        <v>325</v>
+        <v>473</v>
       </c>
       <c r="F105" s="28"/>
     </row>
     <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="28" t="s">
-        <v>466</v>
+        <v>478</v>
       </c>
       <c r="B106" s="28" t="s">
-        <v>467</v>
+        <v>479</v>
       </c>
       <c r="C106" s="28" t="s">
-        <v>325</v>
+        <v>473</v>
       </c>
       <c r="F106" s="28"/>
     </row>
     <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="28" t="s">
-        <v>468</v>
+        <v>195</v>
       </c>
       <c r="B107" s="28" t="s">
-        <v>469</v>
+        <v>480</v>
       </c>
       <c r="C107" s="28" t="s">
-        <v>325</v>
+        <v>481</v>
       </c>
       <c r="F107" s="28"/>
     </row>
     <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="28" t="s">
-        <v>470</v>
+        <v>482</v>
       </c>
       <c r="B108" s="28" t="s">
-        <v>471</v>
+        <v>483</v>
       </c>
       <c r="C108" s="28" t="s">
-        <v>331</v>
+        <v>481</v>
       </c>
       <c r="F108" s="28"/>
     </row>
     <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="28" t="s">
-        <v>472</v>
+        <v>484</v>
       </c>
       <c r="B109" s="28" t="s">
-        <v>473</v>
+        <v>485</v>
       </c>
       <c r="C109" s="28" t="s">
-        <v>325</v>
+        <v>481</v>
       </c>
       <c r="F109" s="28"/>
     </row>
     <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="28" t="s">
-        <v>474</v>
+        <v>486</v>
       </c>
       <c r="B110" s="28" t="s">
-        <v>475</v>
+        <v>487</v>
       </c>
       <c r="C110" s="28" t="s">
-        <v>325</v>
+        <v>481</v>
       </c>
       <c r="F110" s="28"/>
     </row>
     <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="28" t="s">
-        <v>476</v>
+        <v>194</v>
       </c>
       <c r="B111" s="28" t="s">
-        <v>477</v>
+        <v>488</v>
       </c>
       <c r="C111" s="28" t="s">
-        <v>274</v>
+        <v>481</v>
       </c>
       <c r="F111" s="28"/>
     </row>
     <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="28" t="s">
-        <v>478</v>
+        <v>489</v>
       </c>
       <c r="B112" s="28" t="s">
-        <v>479</v>
+        <v>490</v>
       </c>
       <c r="C112" s="28" t="s">
-        <v>331</v>
+        <v>473</v>
       </c>
       <c r="F112" s="28"/>
     </row>
     <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="28" t="s">
-        <v>480</v>
+        <v>491</v>
       </c>
       <c r="B113" s="28" t="s">
-        <v>481</v>
+        <v>492</v>
       </c>
       <c r="C113" s="28" t="s">
-        <v>325</v>
+        <v>473</v>
       </c>
       <c r="F113" s="28"/>
     </row>
     <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="28" t="s">
-        <v>482</v>
+        <v>493</v>
       </c>
       <c r="B114" s="28" t="s">
-        <v>483</v>
+        <v>494</v>
       </c>
       <c r="C114" s="28" t="s">
-        <v>331</v>
+        <v>473</v>
       </c>
       <c r="F114" s="28"/>
     </row>
     <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="28" t="s">
-        <v>484</v>
+        <v>495</v>
       </c>
       <c r="B115" s="28" t="s">
-        <v>485</v>
+        <v>496</v>
       </c>
       <c r="C115" s="28" t="s">
-        <v>274</v>
+        <v>325</v>
       </c>
       <c r="F115" s="28"/>
     </row>
     <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="28" t="s">
-        <v>486</v>
+        <v>497</v>
       </c>
       <c r="B116" s="28" t="s">
-        <v>487</v>
+        <v>498</v>
       </c>
       <c r="C116" s="28" t="s">
-        <v>325</v>
+        <v>331</v>
       </c>
       <c r="F116" s="28"/>
     </row>
     <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="28" t="s">
-        <v>488</v>
+        <v>499</v>
       </c>
       <c r="B117" s="28" t="s">
-        <v>489</v>
+        <v>500</v>
       </c>
       <c r="C117" s="28" t="s">
-        <v>331</v>
+        <v>274</v>
       </c>
       <c r="F117" s="28"/>
     </row>
     <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="28" t="s">
-        <v>490</v>
+        <v>501</v>
       </c>
       <c r="B118" s="28" t="s">
-        <v>491</v>
+        <v>502</v>
       </c>
       <c r="C118" s="28" t="s">
-        <v>424</v>
+        <v>274</v>
       </c>
       <c r="F118" s="28"/>
     </row>
     <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="28" t="s">
-        <v>492</v>
+        <v>503</v>
       </c>
       <c r="B119" s="28" t="s">
-        <v>492</v>
+        <v>504</v>
       </c>
       <c r="C119" s="28" t="s">
-        <v>290</v>
+        <v>331</v>
       </c>
       <c r="F119" s="28"/>
     </row>
     <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="28" t="s">
-        <v>493</v>
+        <v>505</v>
       </c>
       <c r="B120" s="28" t="s">
-        <v>494</v>
+        <v>506</v>
       </c>
       <c r="C120" s="28" t="s">
-        <v>325</v>
+        <v>331</v>
       </c>
       <c r="F120" s="28"/>
     </row>
     <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="28" t="s">
-        <v>495</v>
+        <v>507</v>
       </c>
       <c r="B121" s="28" t="s">
-        <v>496</v>
+        <v>508</v>
       </c>
       <c r="C121" s="28" t="s">
-        <v>274</v>
+        <v>331</v>
       </c>
       <c r="F121" s="28"/>
     </row>
     <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="28" t="s">
-        <v>497</v>
+        <v>509</v>
       </c>
       <c r="B122" s="28" t="s">
-        <v>498</v>
+        <v>510</v>
       </c>
       <c r="C122" s="28" t="s">
-        <v>325</v>
+        <v>331</v>
       </c>
       <c r="F122" s="28"/>
     </row>
     <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="28" t="s">
-        <v>499</v>
+        <v>511</v>
       </c>
       <c r="B123" s="28" t="s">
-        <v>500</v>
+        <v>512</v>
       </c>
       <c r="C123" s="28" t="s">
-        <v>331</v>
+        <v>325</v>
       </c>
       <c r="F123" s="28"/>
     </row>
     <row r="124" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="28" t="s">
-        <v>501</v>
+        <v>513</v>
       </c>
       <c r="B124" s="28" t="s">
-        <v>502</v>
+        <v>514</v>
       </c>
       <c r="C124" s="28" t="s">
-        <v>248</v>
+        <v>325</v>
       </c>
       <c r="F124" s="28"/>
     </row>
     <row r="125" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="28" t="s">
-        <v>503</v>
+        <v>515</v>
       </c>
       <c r="B125" s="28" t="s">
-        <v>504</v>
+        <v>516</v>
       </c>
       <c r="C125" s="28" t="s">
-        <v>331</v>
+        <v>325</v>
       </c>
       <c r="F125" s="28"/>
     </row>
     <row r="126" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="28" t="s">
-        <v>505</v>
+        <v>517</v>
       </c>
       <c r="B126" s="28" t="s">
-        <v>506</v>
+        <v>518</v>
       </c>
       <c r="C126" s="28" t="s">
-        <v>331</v>
+        <v>325</v>
       </c>
       <c r="F126" s="28"/>
     </row>
     <row r="127" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="28" t="s">
-        <v>507</v>
+        <v>519</v>
       </c>
       <c r="B127" s="28" t="s">
-        <v>508</v>
+        <v>520</v>
       </c>
       <c r="C127" s="28" t="s">
         <v>331</v>
@@ -7135,22 +7635,22 @@
     </row>
     <row r="128" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="28" t="s">
-        <v>509</v>
+        <v>521</v>
       </c>
       <c r="B128" s="28" t="s">
-        <v>510</v>
+        <v>522</v>
       </c>
       <c r="C128" s="28" t="s">
-        <v>331</v>
+        <v>325</v>
       </c>
       <c r="F128" s="28"/>
     </row>
     <row r="129" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="28" t="s">
-        <v>237</v>
+        <v>523</v>
       </c>
       <c r="B129" s="28" t="s">
-        <v>511</v>
+        <v>524</v>
       </c>
       <c r="C129" s="28" t="s">
         <v>325</v>
@@ -7159,87 +7659,315 @@
     </row>
     <row r="130" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="28" t="s">
-        <v>512</v>
+        <v>525</v>
       </c>
       <c r="B130" s="28" t="s">
-        <v>513</v>
+        <v>526</v>
       </c>
       <c r="C130" s="28" t="s">
-        <v>331</v>
+        <v>274</v>
       </c>
       <c r="F130" s="28"/>
     </row>
     <row r="131" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="28" t="s">
-        <v>514</v>
+        <v>527</v>
       </c>
       <c r="B131" s="28" t="s">
-        <v>515</v>
+        <v>528</v>
       </c>
       <c r="C131" s="28" t="s">
-        <v>248</v>
+        <v>331</v>
       </c>
       <c r="F131" s="28"/>
     </row>
     <row r="132" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="28" t="s">
-        <v>168</v>
+        <v>529</v>
       </c>
       <c r="B132" s="28" t="s">
-        <v>516</v>
+        <v>530</v>
       </c>
       <c r="C132" s="28" t="s">
-        <v>248</v>
+        <v>325</v>
       </c>
       <c r="F132" s="28"/>
     </row>
     <row r="133" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="28" t="s">
-        <v>517</v>
+        <v>531</v>
       </c>
       <c r="B133" s="28" t="s">
-        <v>518</v>
+        <v>532</v>
       </c>
       <c r="C133" s="28" t="s">
-        <v>248</v>
+        <v>331</v>
       </c>
       <c r="F133" s="28"/>
     </row>
     <row r="134" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="28" t="s">
-        <v>238</v>
+        <v>533</v>
       </c>
       <c r="B134" s="28" t="s">
-        <v>519</v>
+        <v>534</v>
       </c>
       <c r="C134" s="28" t="s">
-        <v>325</v>
+        <v>274</v>
       </c>
       <c r="F134" s="28"/>
     </row>
     <row r="135" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="28" t="s">
-        <v>217</v>
+        <v>535</v>
       </c>
       <c r="B135" s="28" t="s">
-        <v>520</v>
+        <v>536</v>
       </c>
       <c r="C135" s="28" t="s">
-        <v>274</v>
+        <v>325</v>
       </c>
       <c r="F135" s="28"/>
     </row>
     <row r="136" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="28" t="s">
-        <v>521</v>
+        <v>537</v>
       </c>
       <c r="B136" s="28" t="s">
-        <v>522</v>
+        <v>538</v>
       </c>
       <c r="C136" s="28" t="s">
+        <v>331</v>
+      </c>
+      <c r="F136" s="28"/>
+    </row>
+    <row r="137" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A137" s="28" t="s">
+        <v>539</v>
+      </c>
+      <c r="B137" s="28" t="s">
+        <v>540</v>
+      </c>
+      <c r="C137" s="28" t="s">
+        <v>473</v>
+      </c>
+      <c r="F137" s="28"/>
+    </row>
+    <row r="138" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A138" s="28" t="s">
+        <v>541</v>
+      </c>
+      <c r="B138" s="28" t="s">
+        <v>541</v>
+      </c>
+      <c r="C138" s="28" t="s">
+        <v>290</v>
+      </c>
+      <c r="F138" s="28"/>
+    </row>
+    <row r="139" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A139" s="28" t="s">
+        <v>542</v>
+      </c>
+      <c r="B139" s="28" t="s">
+        <v>543</v>
+      </c>
+      <c r="C139" s="28" t="s">
         <v>325</v>
       </c>
-      <c r="F136" s="28"/>
+      <c r="F139" s="28"/>
+    </row>
+    <row r="140" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A140" s="28" t="s">
+        <v>544</v>
+      </c>
+      <c r="B140" s="28" t="s">
+        <v>545</v>
+      </c>
+      <c r="C140" s="28" t="s">
+        <v>274</v>
+      </c>
+      <c r="F140" s="28"/>
+    </row>
+    <row r="141" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A141" s="28" t="s">
+        <v>546</v>
+      </c>
+      <c r="B141" s="28" t="s">
+        <v>547</v>
+      </c>
+      <c r="C141" s="28" t="s">
+        <v>325</v>
+      </c>
+      <c r="F141" s="28"/>
+    </row>
+    <row r="142" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A142" s="28" t="s">
+        <v>548</v>
+      </c>
+      <c r="B142" s="28" t="s">
+        <v>549</v>
+      </c>
+      <c r="C142" s="28" t="s">
+        <v>331</v>
+      </c>
+      <c r="F142" s="28"/>
+    </row>
+    <row r="143" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A143" s="28" t="s">
+        <v>550</v>
+      </c>
+      <c r="B143" s="28" t="s">
+        <v>551</v>
+      </c>
+      <c r="C143" s="28" t="s">
+        <v>248</v>
+      </c>
+      <c r="F143" s="28"/>
+    </row>
+    <row r="144" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A144" s="28" t="s">
+        <v>552</v>
+      </c>
+      <c r="B144" s="28" t="s">
+        <v>553</v>
+      </c>
+      <c r="C144" s="28" t="s">
+        <v>331</v>
+      </c>
+      <c r="F144" s="28"/>
+    </row>
+    <row r="145" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A145" s="28" t="s">
+        <v>554</v>
+      </c>
+      <c r="B145" s="28" t="s">
+        <v>555</v>
+      </c>
+      <c r="C145" s="28" t="s">
+        <v>331</v>
+      </c>
+      <c r="F145" s="28"/>
+    </row>
+    <row r="146" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A146" s="28" t="s">
+        <v>556</v>
+      </c>
+      <c r="B146" s="28" t="s">
+        <v>557</v>
+      </c>
+      <c r="C146" s="28" t="s">
+        <v>331</v>
+      </c>
+      <c r="F146" s="28"/>
+    </row>
+    <row r="147" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A147" s="28" t="s">
+        <v>558</v>
+      </c>
+      <c r="B147" s="28" t="s">
+        <v>559</v>
+      </c>
+      <c r="C147" s="28" t="s">
+        <v>331</v>
+      </c>
+      <c r="F147" s="28"/>
+    </row>
+    <row r="148" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A148" s="28" t="s">
+        <v>237</v>
+      </c>
+      <c r="B148" s="28" t="s">
+        <v>560</v>
+      </c>
+      <c r="C148" s="28" t="s">
+        <v>325</v>
+      </c>
+      <c r="F148" s="28"/>
+    </row>
+    <row r="149" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A149" s="28" t="s">
+        <v>561</v>
+      </c>
+      <c r="B149" s="28" t="s">
+        <v>562</v>
+      </c>
+      <c r="C149" s="28" t="s">
+        <v>331</v>
+      </c>
+      <c r="F149" s="28"/>
+    </row>
+    <row r="150" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A150" s="28" t="s">
+        <v>563</v>
+      </c>
+      <c r="B150" s="28" t="s">
+        <v>564</v>
+      </c>
+      <c r="C150" s="28" t="s">
+        <v>248</v>
+      </c>
+      <c r="F150" s="28"/>
+    </row>
+    <row r="151" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A151" s="28" t="s">
+        <v>168</v>
+      </c>
+      <c r="B151" s="28" t="s">
+        <v>565</v>
+      </c>
+      <c r="C151" s="28" t="s">
+        <v>248</v>
+      </c>
+      <c r="F151" s="28"/>
+    </row>
+    <row r="152" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A152" s="28" t="s">
+        <v>566</v>
+      </c>
+      <c r="B152" s="28" t="s">
+        <v>567</v>
+      </c>
+      <c r="C152" s="28" t="s">
+        <v>248</v>
+      </c>
+      <c r="F152" s="28"/>
+    </row>
+    <row r="153" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A153" s="28" t="s">
+        <v>238</v>
+      </c>
+      <c r="B153" s="28" t="s">
+        <v>568</v>
+      </c>
+      <c r="C153" s="28" t="s">
+        <v>325</v>
+      </c>
+      <c r="F153" s="28"/>
+    </row>
+    <row r="154" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A154" s="28" t="s">
+        <v>217</v>
+      </c>
+      <c r="B154" s="28" t="s">
+        <v>569</v>
+      </c>
+      <c r="C154" s="28" t="s">
+        <v>274</v>
+      </c>
+      <c r="F154" s="28"/>
+    </row>
+    <row r="155" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A155" s="28" t="s">
+        <v>570</v>
+      </c>
+      <c r="B155" s="28" t="s">
+        <v>571</v>
+      </c>
+      <c r="C155" s="28" t="s">
+        <v>325</v>
+      </c>
+      <c r="F155" s="28"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>